<commit_message>
melhorando o modelo de previsao
</commit_message>
<xml_diff>
--- a/saida_final.xlsx
+++ b/saida_final.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -469,10 +473,8 @@
       <c r="A2" t="n">
         <v>120210601</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2021-06-01</t>
-        </is>
+      <c r="B2" s="2" t="n">
+        <v>44348</v>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
@@ -491,10 +493,8 @@
       <c r="A3" t="n">
         <v>220210601</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2021-06-01</t>
-        </is>
+      <c r="B3" s="2" t="n">
+        <v>44348</v>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
@@ -513,10 +513,8 @@
       <c r="A4" t="n">
         <v>320210604</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2021-06-04</t>
-        </is>
+      <c r="B4" s="2" t="n">
+        <v>44351</v>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
@@ -535,10 +533,8 @@
       <c r="A5" t="n">
         <v>420210604</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2021-06-04</t>
-        </is>
+      <c r="B5" s="2" t="n">
+        <v>44351</v>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
@@ -557,10 +553,8 @@
       <c r="A6" t="n">
         <v>420210604</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2021-06-04</t>
-        </is>
+      <c r="B6" s="2" t="n">
+        <v>44351</v>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
@@ -579,10 +573,8 @@
       <c r="A7" t="n">
         <v>520210604</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2021-06-04</t>
-        </is>
+      <c r="B7" s="2" t="n">
+        <v>44351</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
@@ -601,10 +593,8 @@
       <c r="A8" t="n">
         <v>620210604</v>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2021-06-04</t>
-        </is>
+      <c r="B8" s="2" t="n">
+        <v>44351</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
@@ -623,10 +613,8 @@
       <c r="A9" t="n">
         <v>620210605</v>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>2021-06-05</t>
-        </is>
+      <c r="B9" s="2" t="n">
+        <v>44352</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
@@ -645,10 +633,8 @@
       <c r="A10" t="n">
         <v>720210605</v>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>2021-06-05</t>
-        </is>
+      <c r="B10" s="2" t="n">
+        <v>44352</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
@@ -667,10 +653,8 @@
       <c r="A11" t="n">
         <v>820210605</v>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>2021-06-05</t>
-        </is>
+      <c r="B11" s="2" t="n">
+        <v>44352</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
@@ -689,10 +673,8 @@
       <c r="A12" t="n">
         <v>820210606</v>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>2021-06-06</t>
-        </is>
+      <c r="B12" s="2" t="n">
+        <v>44353</v>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
@@ -711,10 +693,8 @@
       <c r="A13" t="n">
         <v>920210606</v>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>2021-06-06</t>
-        </is>
+      <c r="B13" s="2" t="n">
+        <v>44353</v>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
@@ -733,10 +713,8 @@
       <c r="A14" t="n">
         <v>920210606</v>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>2021-06-06</t>
-        </is>
+      <c r="B14" s="2" t="n">
+        <v>44353</v>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
@@ -755,10 +733,8 @@
       <c r="A15" t="n">
         <v>920210607</v>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>2021-06-07</t>
-        </is>
+      <c r="B15" s="2" t="n">
+        <v>44354</v>
       </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr">
@@ -777,10 +753,8 @@
       <c r="A16" t="n">
         <v>920210607</v>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>2021-06-07</t>
-        </is>
+      <c r="B16" s="2" t="n">
+        <v>44354</v>
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr">
@@ -799,10 +773,8 @@
       <c r="A17" t="n">
         <v>1020210609</v>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>2021-06-09</t>
-        </is>
+      <c r="B17" s="2" t="n">
+        <v>44356</v>
       </c>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr">
@@ -821,10 +793,8 @@
       <c r="A18" t="n">
         <v>1120210609</v>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>2021-06-09</t>
-        </is>
+      <c r="B18" s="2" t="n">
+        <v>44356</v>
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr">
@@ -843,10 +813,8 @@
       <c r="A19" t="n">
         <v>1120210609</v>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>2021-06-09</t>
-        </is>
+      <c r="B19" s="2" t="n">
+        <v>44356</v>
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr">
@@ -865,10 +833,8 @@
       <c r="A20" t="n">
         <v>1220210610</v>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>2021-06-10</t>
-        </is>
+      <c r="B20" s="2" t="n">
+        <v>44357</v>
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr">
@@ -887,10 +853,8 @@
       <c r="A21" t="n">
         <v>1220210610</v>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>2021-06-10</t>
-        </is>
+      <c r="B21" s="2" t="n">
+        <v>44357</v>
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr">
@@ -909,10 +873,8 @@
       <c r="A22" t="n">
         <v>1320210611</v>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>2021-06-11</t>
-        </is>
+      <c r="B22" s="2" t="n">
+        <v>44358</v>
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr">
@@ -931,10 +893,8 @@
       <c r="A23" t="n">
         <v>1420210611</v>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>2021-06-11</t>
-        </is>
+      <c r="B23" s="2" t="n">
+        <v>44358</v>
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr">
@@ -953,10 +913,8 @@
       <c r="A24" t="n">
         <v>1420210611</v>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>2021-06-11</t>
-        </is>
+      <c r="B24" s="2" t="n">
+        <v>44358</v>
       </c>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr">
@@ -975,10 +933,8 @@
       <c r="A25" t="n">
         <v>1420210612</v>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>2021-06-12</t>
-        </is>
+      <c r="B25" s="2" t="n">
+        <v>44359</v>
       </c>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr">
@@ -997,10 +953,8 @@
       <c r="A26" t="n">
         <v>1420210612</v>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>2021-06-12</t>
-        </is>
+      <c r="B26" s="2" t="n">
+        <v>44359</v>
       </c>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr">
@@ -1019,10 +973,8 @@
       <c r="A27" t="n">
         <v>1420210612</v>
       </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>2021-06-12</t>
-        </is>
+      <c r="B27" s="2" t="n">
+        <v>44359</v>
       </c>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr">
@@ -1041,10 +993,8 @@
       <c r="A28" t="n">
         <v>1420210613</v>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>2021-06-13</t>
-        </is>
+      <c r="B28" s="2" t="n">
+        <v>44360</v>
       </c>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr">
@@ -1063,10 +1013,8 @@
       <c r="A29" t="n">
         <v>1520210613</v>
       </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>2021-06-13</t>
-        </is>
+      <c r="B29" s="2" t="n">
+        <v>44360</v>
       </c>
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr">
@@ -1085,10 +1033,8 @@
       <c r="A30" t="n">
         <v>1520210613</v>
       </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>2021-06-13</t>
-        </is>
+      <c r="B30" s="2" t="n">
+        <v>44360</v>
       </c>
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr">
@@ -1107,10 +1053,8 @@
       <c r="A31" t="n">
         <v>1520210613</v>
       </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>2021-06-13</t>
-        </is>
+      <c r="B31" s="2" t="n">
+        <v>44360</v>
       </c>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr">
@@ -1129,10 +1073,8 @@
       <c r="A32" t="n">
         <v>1620210613</v>
       </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>2021-06-13</t>
-        </is>
+      <c r="B32" s="2" t="n">
+        <v>44360</v>
       </c>
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr">
@@ -1151,10 +1093,8 @@
       <c r="A33" t="n">
         <v>1620210613</v>
       </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>2021-06-13</t>
-        </is>
+      <c r="B33" s="2" t="n">
+        <v>44360</v>
       </c>
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr">
@@ -1173,10 +1113,8 @@
       <c r="A34" t="n">
         <v>1720210614</v>
       </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>2021-06-14</t>
-        </is>
+      <c r="B34" s="2" t="n">
+        <v>44361</v>
       </c>
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr">
@@ -1195,10 +1133,8 @@
       <c r="A35" t="n">
         <v>1820210614</v>
       </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>2021-06-14</t>
-        </is>
+      <c r="B35" s="2" t="n">
+        <v>44361</v>
       </c>
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr">
@@ -1217,10 +1153,8 @@
       <c r="A36" t="n">
         <v>1820210615</v>
       </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>2021-06-15</t>
-        </is>
+      <c r="B36" s="2" t="n">
+        <v>44362</v>
       </c>
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr">
@@ -1239,10 +1173,8 @@
       <c r="A37" t="n">
         <v>1820210615</v>
       </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>2021-06-15</t>
-        </is>
+      <c r="B37" s="2" t="n">
+        <v>44362</v>
       </c>
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="inlineStr">
@@ -1261,10 +1193,8 @@
       <c r="A38" t="n">
         <v>1820210615</v>
       </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>2021-06-15</t>
-        </is>
+      <c r="B38" s="2" t="n">
+        <v>44362</v>
       </c>
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="inlineStr">
@@ -1283,10 +1213,8 @@
       <c r="A39" t="n">
         <v>1920210618</v>
       </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>2021-06-18</t>
-        </is>
+      <c r="B39" s="2" t="n">
+        <v>44365</v>
       </c>
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="inlineStr">
@@ -1305,10 +1233,8 @@
       <c r="A40" t="n">
         <v>2020210618</v>
       </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>2021-06-18</t>
-        </is>
+      <c r="B40" s="2" t="n">
+        <v>44365</v>
       </c>
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="inlineStr">
@@ -1327,10 +1253,8 @@
       <c r="A41" t="n">
         <v>2120210618</v>
       </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>2021-06-18</t>
-        </is>
+      <c r="B41" s="2" t="n">
+        <v>44365</v>
       </c>
       <c r="C41" t="inlineStr"/>
       <c r="D41" t="inlineStr">
@@ -1349,10 +1273,8 @@
       <c r="A42" t="n">
         <v>2120210618</v>
       </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>2021-06-18</t>
-        </is>
+      <c r="B42" s="2" t="n">
+        <v>44365</v>
       </c>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="inlineStr">
@@ -1371,10 +1293,8 @@
       <c r="A43" t="n">
         <v>2220210618</v>
       </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>2021-06-18</t>
-        </is>
+      <c r="B43" s="2" t="n">
+        <v>44365</v>
       </c>
       <c r="C43" t="inlineStr"/>
       <c r="D43" t="inlineStr">
@@ -1393,10 +1313,8 @@
       <c r="A44" t="n">
         <v>2320210619</v>
       </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>2021-06-19</t>
-        </is>
+      <c r="B44" s="2" t="n">
+        <v>44366</v>
       </c>
       <c r="C44" t="inlineStr"/>
       <c r="D44" t="inlineStr">
@@ -1415,10 +1333,8 @@
       <c r="A45" t="n">
         <v>2420210619</v>
       </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>2021-06-19</t>
-        </is>
+      <c r="B45" s="2" t="n">
+        <v>44366</v>
       </c>
       <c r="C45" t="inlineStr"/>
       <c r="D45" t="inlineStr">
@@ -1437,10 +1353,8 @@
       <c r="A46" t="n">
         <v>2520210619</v>
       </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>2021-06-19</t>
-        </is>
+      <c r="B46" s="2" t="n">
+        <v>44366</v>
       </c>
       <c r="C46" t="inlineStr"/>
       <c r="D46" t="inlineStr">
@@ -1459,10 +1373,8 @@
       <c r="A47" t="n">
         <v>2620210620</v>
       </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>2021-06-20</t>
-        </is>
+      <c r="B47" s="2" t="n">
+        <v>44367</v>
       </c>
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="inlineStr">
@@ -1481,10 +1393,8 @@
       <c r="A48" t="n">
         <v>2720210620</v>
       </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>2021-06-20</t>
-        </is>
+      <c r="B48" s="2" t="n">
+        <v>44367</v>
       </c>
       <c r="C48" t="inlineStr"/>
       <c r="D48" t="inlineStr">
@@ -1503,10 +1413,8 @@
       <c r="A49" t="n">
         <v>2820210620</v>
       </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>2021-06-20</t>
-        </is>
+      <c r="B49" s="2" t="n">
+        <v>44367</v>
       </c>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr">
@@ -1525,10 +1433,8 @@
       <c r="A50" t="n">
         <v>2820210620</v>
       </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>2021-06-20</t>
-        </is>
+      <c r="B50" s="2" t="n">
+        <v>44367</v>
       </c>
       <c r="C50" t="inlineStr"/>
       <c r="D50" t="inlineStr">
@@ -1547,10 +1453,8 @@
       <c r="A51" t="n">
         <v>2920210620</v>
       </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>2021-06-20</t>
-        </is>
+      <c r="B51" s="2" t="n">
+        <v>44367</v>
       </c>
       <c r="C51" t="inlineStr"/>
       <c r="D51" t="inlineStr">
@@ -1569,10 +1473,8 @@
       <c r="A52" t="n">
         <v>2920210620</v>
       </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>2021-06-20</t>
-        </is>
+      <c r="B52" s="2" t="n">
+        <v>44367</v>
       </c>
       <c r="C52" t="inlineStr"/>
       <c r="D52" t="inlineStr">
@@ -1591,10 +1493,8 @@
       <c r="A53" t="n">
         <v>3020210622</v>
       </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>2021-06-22</t>
-        </is>
+      <c r="B53" s="2" t="n">
+        <v>44369</v>
       </c>
       <c r="C53" t="inlineStr"/>
       <c r="D53" t="inlineStr">
@@ -1613,10 +1513,8 @@
       <c r="A54" t="n">
         <v>3020210622</v>
       </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>2021-06-22</t>
-        </is>
+      <c r="B54" s="2" t="n">
+        <v>44369</v>
       </c>
       <c r="C54" t="inlineStr"/>
       <c r="D54" t="inlineStr">
@@ -1635,10 +1533,8 @@
       <c r="A55" t="n">
         <v>3020210622</v>
       </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>2021-06-22</t>
-        </is>
+      <c r="B55" s="2" t="n">
+        <v>44369</v>
       </c>
       <c r="C55" t="inlineStr"/>
       <c r="D55" t="inlineStr">
@@ -1657,10 +1553,8 @@
       <c r="A56" t="n">
         <v>3020210623</v>
       </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>2021-06-23</t>
-        </is>
+      <c r="B56" s="2" t="n">
+        <v>44370</v>
       </c>
       <c r="C56" t="inlineStr"/>
       <c r="D56" t="inlineStr">
@@ -1679,10 +1573,8 @@
       <c r="A57" t="n">
         <v>3120210623</v>
       </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>2021-06-23</t>
-        </is>
+      <c r="B57" s="2" t="n">
+        <v>44370</v>
       </c>
       <c r="C57" t="inlineStr"/>
       <c r="D57" t="inlineStr">
@@ -1701,10 +1593,8 @@
       <c r="A58" t="n">
         <v>3120210623</v>
       </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>2021-06-23</t>
-        </is>
+      <c r="B58" s="2" t="n">
+        <v>44370</v>
       </c>
       <c r="C58" t="inlineStr"/>
       <c r="D58" t="inlineStr">
@@ -1723,10 +1613,8 @@
       <c r="A59" t="n">
         <v>3120210625</v>
       </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>2021-06-25</t>
-        </is>
+      <c r="B59" s="2" t="n">
+        <v>44372</v>
       </c>
       <c r="C59" t="inlineStr"/>
       <c r="D59" t="inlineStr">
@@ -1745,10 +1633,8 @@
       <c r="A60" t="n">
         <v>3120210625</v>
       </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>2021-06-25</t>
-        </is>
+      <c r="B60" s="2" t="n">
+        <v>44372</v>
       </c>
       <c r="C60" t="inlineStr"/>
       <c r="D60" t="inlineStr">
@@ -1767,10 +1653,8 @@
       <c r="A61" t="n">
         <v>3220210625</v>
       </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>2021-06-25</t>
-        </is>
+      <c r="B61" s="2" t="n">
+        <v>44372</v>
       </c>
       <c r="C61" t="inlineStr"/>
       <c r="D61" t="inlineStr">
@@ -1789,10 +1673,8 @@
       <c r="A62" t="n">
         <v>3320210625</v>
       </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>2021-06-25</t>
-        </is>
+      <c r="B62" s="2" t="n">
+        <v>44372</v>
       </c>
       <c r="C62" t="inlineStr"/>
       <c r="D62" t="inlineStr">
@@ -1811,10 +1693,8 @@
       <c r="A63" t="n">
         <v>3320210625</v>
       </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>2021-06-25</t>
-        </is>
+      <c r="B63" s="2" t="n">
+        <v>44372</v>
       </c>
       <c r="C63" t="inlineStr"/>
       <c r="D63" t="inlineStr">
@@ -1833,10 +1713,8 @@
       <c r="A64" t="n">
         <v>3320210626</v>
       </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>2021-06-26</t>
-        </is>
+      <c r="B64" s="2" t="n">
+        <v>44373</v>
       </c>
       <c r="C64" t="inlineStr"/>
       <c r="D64" t="inlineStr">
@@ -1855,10 +1733,8 @@
       <c r="A65" t="n">
         <v>3320210626</v>
       </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>2021-06-26</t>
-        </is>
+      <c r="B65" s="2" t="n">
+        <v>44373</v>
       </c>
       <c r="C65" t="inlineStr"/>
       <c r="D65" t="inlineStr">
@@ -1877,10 +1753,8 @@
       <c r="A66" t="n">
         <v>3320210626</v>
       </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>2021-06-26</t>
-        </is>
+      <c r="B66" s="2" t="n">
+        <v>44373</v>
       </c>
       <c r="C66" t="inlineStr"/>
       <c r="D66" t="inlineStr">
@@ -1899,10 +1773,8 @@
       <c r="A67" t="n">
         <v>3420210626</v>
       </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>2021-06-26</t>
-        </is>
+      <c r="B67" s="2" t="n">
+        <v>44373</v>
       </c>
       <c r="C67" t="inlineStr"/>
       <c r="D67" t="inlineStr">
@@ -1921,10 +1793,8 @@
       <c r="A68" t="n">
         <v>3520210626</v>
       </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>2021-06-26</t>
-        </is>
+      <c r="B68" s="2" t="n">
+        <v>44373</v>
       </c>
       <c r="C68" t="inlineStr"/>
       <c r="D68" t="inlineStr">
@@ -1943,10 +1813,8 @@
       <c r="A69" t="n">
         <v>3620210626</v>
       </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>2021-06-26</t>
-        </is>
+      <c r="B69" s="2" t="n">
+        <v>44373</v>
       </c>
       <c r="C69" t="inlineStr"/>
       <c r="D69" t="inlineStr">
@@ -1965,10 +1833,8 @@
       <c r="A70" t="n">
         <v>3720210627</v>
       </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>2021-06-27</t>
-        </is>
+      <c r="B70" s="2" t="n">
+        <v>44374</v>
       </c>
       <c r="C70" t="inlineStr"/>
       <c r="D70" t="inlineStr">
@@ -1987,10 +1853,8 @@
       <c r="A71" t="n">
         <v>3820210627</v>
       </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>2021-06-27</t>
-        </is>
+      <c r="B71" s="2" t="n">
+        <v>44374</v>
       </c>
       <c r="C71" t="inlineStr"/>
       <c r="D71" t="inlineStr">
@@ -2009,10 +1873,8 @@
       <c r="A72" t="n">
         <v>3920210627</v>
       </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>2021-06-27</t>
-        </is>
+      <c r="B72" s="2" t="n">
+        <v>44374</v>
       </c>
       <c r="C72" t="inlineStr"/>
       <c r="D72" t="inlineStr">
@@ -2031,10 +1893,8 @@
       <c r="A73" t="n">
         <v>3920210627</v>
       </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>2021-06-27</t>
-        </is>
+      <c r="B73" s="2" t="n">
+        <v>44374</v>
       </c>
       <c r="C73" t="inlineStr"/>
       <c r="D73" t="inlineStr">
@@ -2053,10 +1913,8 @@
       <c r="A74" t="n">
         <v>4020210627</v>
       </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>2021-06-27</t>
-        </is>
+      <c r="B74" s="2" t="n">
+        <v>44374</v>
       </c>
       <c r="C74" t="inlineStr"/>
       <c r="D74" t="inlineStr">
@@ -2075,10 +1933,8 @@
       <c r="A75" t="n">
         <v>4120210627</v>
       </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>2021-06-27</t>
-        </is>
+      <c r="B75" s="2" t="n">
+        <v>44374</v>
       </c>
       <c r="C75" t="inlineStr"/>
       <c r="D75" t="inlineStr">
@@ -2097,10 +1953,8 @@
       <c r="A76" t="n">
         <v>4220210628</v>
       </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>2021-06-28</t>
-        </is>
+      <c r="B76" s="2" t="n">
+        <v>44375</v>
       </c>
       <c r="C76" t="inlineStr"/>
       <c r="D76" t="inlineStr">
@@ -2119,10 +1973,8 @@
       <c r="A77" t="n">
         <v>4220210628</v>
       </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>2021-06-28</t>
-        </is>
+      <c r="B77" s="2" t="n">
+        <v>44375</v>
       </c>
       <c r="C77" t="inlineStr"/>
       <c r="D77" t="inlineStr">
@@ -2141,10 +1993,8 @@
       <c r="A78" t="n">
         <v>4320210629</v>
       </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>2021-06-29</t>
-        </is>
+      <c r="B78" s="2" t="n">
+        <v>44376</v>
       </c>
       <c r="C78" t="inlineStr"/>
       <c r="D78" t="inlineStr">
@@ -2163,10 +2013,8 @@
       <c r="A79" t="n">
         <v>4320210629</v>
       </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>2021-06-29</t>
-        </is>
+      <c r="B79" s="2" t="n">
+        <v>44376</v>
       </c>
       <c r="C79" t="inlineStr"/>
       <c r="D79" t="inlineStr">
@@ -2185,10 +2033,8 @@
       <c r="A80" t="n">
         <v>4420210629</v>
       </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>2021-06-29</t>
-        </is>
+      <c r="B80" s="2" t="n">
+        <v>44376</v>
       </c>
       <c r="C80" t="inlineStr"/>
       <c r="D80" t="inlineStr">
@@ -2207,10 +2053,8 @@
       <c r="A81" t="n">
         <v>4520210630</v>
       </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>2021-06-30</t>
-        </is>
+      <c r="B81" s="2" t="n">
+        <v>44377</v>
       </c>
       <c r="C81" t="inlineStr"/>
       <c r="D81" t="inlineStr">
@@ -2229,10 +2073,8 @@
       <c r="A82" t="n">
         <v>4520210630</v>
       </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>2021-06-30</t>
-        </is>
+      <c r="B82" s="2" t="n">
+        <v>44377</v>
       </c>
       <c r="C82" t="inlineStr"/>
       <c r="D82" t="inlineStr">
@@ -2251,10 +2093,8 @@
       <c r="A83" t="n">
         <v>4520210630</v>
       </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>2021-06-30</t>
-        </is>
+      <c r="B83" s="2" t="n">
+        <v>44377</v>
       </c>
       <c r="C83" t="inlineStr"/>
       <c r="D83" t="inlineStr">
@@ -2273,10 +2113,8 @@
       <c r="A84" t="n">
         <v>4520210701</v>
       </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>2021-07-01</t>
-        </is>
+      <c r="B84" s="2" t="n">
+        <v>44378</v>
       </c>
       <c r="C84" t="inlineStr"/>
       <c r="D84" t="inlineStr">
@@ -2295,10 +2133,8 @@
       <c r="A85" t="n">
         <v>4620210701</v>
       </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>2021-07-01</t>
-        </is>
+      <c r="B85" s="2" t="n">
+        <v>44378</v>
       </c>
       <c r="C85" t="inlineStr"/>
       <c r="D85" t="inlineStr">
@@ -2317,10 +2153,8 @@
       <c r="A86" t="n">
         <v>4720210702</v>
       </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>2021-07-02</t>
-        </is>
+      <c r="B86" s="2" t="n">
+        <v>44379</v>
       </c>
       <c r="C86" t="inlineStr"/>
       <c r="D86" t="inlineStr">
@@ -2339,10 +2173,8 @@
       <c r="A87" t="n">
         <v>4720210702</v>
       </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>2021-07-02</t>
-        </is>
+      <c r="B87" s="2" t="n">
+        <v>44379</v>
       </c>
       <c r="C87" t="inlineStr"/>
       <c r="D87" t="inlineStr">
@@ -2361,10 +2193,8 @@
       <c r="A88" t="n">
         <v>4820210702</v>
       </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>2021-07-02</t>
-        </is>
+      <c r="B88" s="2" t="n">
+        <v>44379</v>
       </c>
       <c r="C88" t="inlineStr"/>
       <c r="D88" t="inlineStr">
@@ -2383,10 +2213,8 @@
       <c r="A89" t="n">
         <v>4920210702</v>
       </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>2021-07-02</t>
-        </is>
+      <c r="B89" s="2" t="n">
+        <v>44379</v>
       </c>
       <c r="C89" t="inlineStr"/>
       <c r="D89" t="inlineStr">
@@ -2405,10 +2233,8 @@
       <c r="A90" t="n">
         <v>4920210703</v>
       </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>2021-07-03</t>
-        </is>
+      <c r="B90" s="2" t="n">
+        <v>44380</v>
       </c>
       <c r="C90" t="inlineStr"/>
       <c r="D90" t="inlineStr">
@@ -2427,10 +2253,8 @@
       <c r="A91" t="n">
         <v>4920210703</v>
       </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>2021-07-03</t>
-        </is>
+      <c r="B91" s="2" t="n">
+        <v>44380</v>
       </c>
       <c r="C91" t="inlineStr"/>
       <c r="D91" t="inlineStr">
@@ -2449,10 +2273,8 @@
       <c r="A92" t="n">
         <v>5020210703</v>
       </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>2021-07-03</t>
-        </is>
+      <c r="B92" s="2" t="n">
+        <v>44380</v>
       </c>
       <c r="C92" t="inlineStr"/>
       <c r="D92" t="inlineStr">
@@ -2471,10 +2293,8 @@
       <c r="A93" t="n">
         <v>5120210703</v>
       </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>2021-07-03</t>
-        </is>
+      <c r="B93" s="2" t="n">
+        <v>44380</v>
       </c>
       <c r="C93" t="inlineStr"/>
       <c r="D93" t="inlineStr">
@@ -2493,10 +2313,8 @@
       <c r="A94" t="n">
         <v>5220210703</v>
       </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>2021-07-03</t>
-        </is>
+      <c r="B94" s="2" t="n">
+        <v>44380</v>
       </c>
       <c r="C94" t="inlineStr"/>
       <c r="D94" t="inlineStr">
@@ -2515,10 +2333,8 @@
       <c r="A95" t="n">
         <v>5320210703</v>
       </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>2021-07-03</t>
-        </is>
+      <c r="B95" s="2" t="n">
+        <v>44380</v>
       </c>
       <c r="C95" t="inlineStr"/>
       <c r="D95" t="inlineStr">
@@ -2537,10 +2353,8 @@
       <c r="A96" t="n">
         <v>5320210704</v>
       </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>2021-07-04</t>
-        </is>
+      <c r="B96" s="2" t="n">
+        <v>44381</v>
       </c>
       <c r="C96" t="inlineStr"/>
       <c r="D96" t="inlineStr">
@@ -2559,10 +2373,8 @@
       <c r="A97" t="n">
         <v>5320210704</v>
       </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>2021-07-04</t>
-        </is>
+      <c r="B97" s="2" t="n">
+        <v>44381</v>
       </c>
       <c r="C97" t="inlineStr"/>
       <c r="D97" t="inlineStr">
@@ -2581,10 +2393,8 @@
       <c r="A98" t="n">
         <v>5320210704</v>
       </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>2021-07-04</t>
-        </is>
+      <c r="B98" s="2" t="n">
+        <v>44381</v>
       </c>
       <c r="C98" t="inlineStr"/>
       <c r="D98" t="inlineStr">
@@ -2603,10 +2413,8 @@
       <c r="A99" t="n">
         <v>5320210705</v>
       </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>2021-07-05</t>
-        </is>
+      <c r="B99" s="2" t="n">
+        <v>44382</v>
       </c>
       <c r="C99" t="inlineStr"/>
       <c r="D99" t="inlineStr">
@@ -2625,10 +2433,8 @@
       <c r="A100" t="n">
         <v>5320210705</v>
       </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>2021-07-05</t>
-        </is>
+      <c r="B100" s="2" t="n">
+        <v>44382</v>
       </c>
       <c r="C100" t="inlineStr"/>
       <c r="D100" t="inlineStr">
@@ -2647,10 +2453,8 @@
       <c r="A101" t="n">
         <v>5320210705</v>
       </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>2021-07-05</t>
-        </is>
+      <c r="B101" s="2" t="n">
+        <v>44382</v>
       </c>
       <c r="C101" t="inlineStr"/>
       <c r="D101" t="inlineStr">
@@ -2669,10 +2473,8 @@
       <c r="A102" t="n">
         <v>5320210706</v>
       </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>2021-07-06</t>
-        </is>
+      <c r="B102" s="2" t="n">
+        <v>44383</v>
       </c>
       <c r="C102" t="inlineStr"/>
       <c r="D102" t="inlineStr">
@@ -2691,10 +2493,8 @@
       <c r="A103" t="n">
         <v>5420210706</v>
       </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>2021-07-06</t>
-        </is>
+      <c r="B103" s="2" t="n">
+        <v>44383</v>
       </c>
       <c r="C103" t="inlineStr"/>
       <c r="D103" t="inlineStr">
@@ -2713,10 +2513,8 @@
       <c r="A104" t="n">
         <v>5420210706</v>
       </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>2021-07-06</t>
-        </is>
+      <c r="B104" s="2" t="n">
+        <v>44383</v>
       </c>
       <c r="C104" t="inlineStr"/>
       <c r="D104" t="inlineStr">
@@ -2735,10 +2533,8 @@
       <c r="A105" t="n">
         <v>5420210706</v>
       </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>2021-07-06</t>
-        </is>
+      <c r="B105" s="2" t="n">
+        <v>44383</v>
       </c>
       <c r="C105" t="inlineStr"/>
       <c r="D105" t="inlineStr">
@@ -2757,10 +2553,8 @@
       <c r="A106" t="n">
         <v>5520210707</v>
       </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>2021-07-07</t>
-        </is>
+      <c r="B106" s="2" t="n">
+        <v>44384</v>
       </c>
       <c r="C106" t="inlineStr"/>
       <c r="D106" t="inlineStr">
@@ -2779,10 +2573,8 @@
       <c r="A107" t="n">
         <v>5520210707</v>
       </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>2021-07-07</t>
-        </is>
+      <c r="B107" s="2" t="n">
+        <v>44384</v>
       </c>
       <c r="C107" t="inlineStr"/>
       <c r="D107" t="inlineStr">
@@ -2801,10 +2593,8 @@
       <c r="A108" t="n">
         <v>5520210707</v>
       </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>2021-07-07</t>
-        </is>
+      <c r="B108" s="2" t="n">
+        <v>44384</v>
       </c>
       <c r="C108" t="inlineStr"/>
       <c r="D108" t="inlineStr">
@@ -2823,10 +2613,8 @@
       <c r="A109" t="n">
         <v>5520210708</v>
       </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>2021-07-08</t>
-        </is>
+      <c r="B109" s="2" t="n">
+        <v>44385</v>
       </c>
       <c r="C109" t="inlineStr"/>
       <c r="D109" t="inlineStr">
@@ -2845,10 +2633,8 @@
       <c r="A110" t="n">
         <v>5620210708</v>
       </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>2021-07-08</t>
-        </is>
+      <c r="B110" s="2" t="n">
+        <v>44385</v>
       </c>
       <c r="C110" t="inlineStr"/>
       <c r="D110" t="inlineStr">
@@ -2867,10 +2653,8 @@
       <c r="A111" t="n">
         <v>5620210708</v>
       </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>2021-07-08</t>
-        </is>
+      <c r="B111" s="2" t="n">
+        <v>44385</v>
       </c>
       <c r="C111" t="inlineStr"/>
       <c r="D111" t="inlineStr">
@@ -2889,10 +2673,8 @@
       <c r="A112" t="n">
         <v>5620210709</v>
       </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>2021-07-09</t>
-        </is>
+      <c r="B112" s="2" t="n">
+        <v>44386</v>
       </c>
       <c r="C112" t="inlineStr"/>
       <c r="D112" t="inlineStr">
@@ -2911,10 +2693,8 @@
       <c r="A113" t="n">
         <v>5620210709</v>
       </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>2021-07-09</t>
-        </is>
+      <c r="B113" s="2" t="n">
+        <v>44386</v>
       </c>
       <c r="C113" t="inlineStr"/>
       <c r="D113" t="inlineStr">
@@ -2933,10 +2713,8 @@
       <c r="A114" t="n">
         <v>5720210709</v>
       </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>2021-07-09</t>
-        </is>
+      <c r="B114" s="2" t="n">
+        <v>44386</v>
       </c>
       <c r="C114" t="inlineStr"/>
       <c r="D114" t="inlineStr">
@@ -2955,10 +2733,8 @@
       <c r="A115" t="n">
         <v>5820210709</v>
       </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>2021-07-09</t>
-        </is>
+      <c r="B115" s="2" t="n">
+        <v>44386</v>
       </c>
       <c r="C115" t="inlineStr"/>
       <c r="D115" t="inlineStr">
@@ -2977,10 +2753,8 @@
       <c r="A116" t="n">
         <v>5920210709</v>
       </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>2021-07-09</t>
-        </is>
+      <c r="B116" s="2" t="n">
+        <v>44386</v>
       </c>
       <c r="C116" t="inlineStr"/>
       <c r="D116" t="inlineStr">
@@ -2999,10 +2773,8 @@
       <c r="A117" t="n">
         <v>6020210710</v>
       </c>
-      <c r="B117" t="inlineStr">
-        <is>
-          <t>2021-07-10</t>
-        </is>
+      <c r="B117" s="2" t="n">
+        <v>44387</v>
       </c>
       <c r="C117" t="inlineStr"/>
       <c r="D117" t="inlineStr">
@@ -3021,10 +2793,8 @@
       <c r="A118" t="n">
         <v>6020210710</v>
       </c>
-      <c r="B118" t="inlineStr">
-        <is>
-          <t>2021-07-10</t>
-        </is>
+      <c r="B118" s="2" t="n">
+        <v>44387</v>
       </c>
       <c r="C118" t="inlineStr"/>
       <c r="D118" t="inlineStr">
@@ -3043,10 +2813,8 @@
       <c r="A119" t="n">
         <v>6020210710</v>
       </c>
-      <c r="B119" t="inlineStr">
-        <is>
-          <t>2021-07-10</t>
-        </is>
+      <c r="B119" s="2" t="n">
+        <v>44387</v>
       </c>
       <c r="C119" t="inlineStr"/>
       <c r="D119" t="inlineStr">
@@ -3065,10 +2833,8 @@
       <c r="A120" t="n">
         <v>6120210710</v>
       </c>
-      <c r="B120" t="inlineStr">
-        <is>
-          <t>2021-07-10</t>
-        </is>
+      <c r="B120" s="2" t="n">
+        <v>44387</v>
       </c>
       <c r="C120" t="inlineStr"/>
       <c r="D120" t="inlineStr">
@@ -3087,10 +2853,8 @@
       <c r="A121" t="n">
         <v>6220210710</v>
       </c>
-      <c r="B121" t="inlineStr">
-        <is>
-          <t>2021-07-10</t>
-        </is>
+      <c r="B121" s="2" t="n">
+        <v>44387</v>
       </c>
       <c r="C121" t="inlineStr"/>
       <c r="D121" t="inlineStr">
@@ -3109,10 +2873,8 @@
       <c r="A122" t="n">
         <v>6220210710</v>
       </c>
-      <c r="B122" t="inlineStr">
-        <is>
-          <t>2021-07-10</t>
-        </is>
+      <c r="B122" s="2" t="n">
+        <v>44387</v>
       </c>
       <c r="C122" t="inlineStr"/>
       <c r="D122" t="inlineStr">
@@ -3131,10 +2893,8 @@
       <c r="A123" t="n">
         <v>6320210711</v>
       </c>
-      <c r="B123" t="inlineStr">
-        <is>
-          <t>2021-07-11</t>
-        </is>
+      <c r="B123" s="2" t="n">
+        <v>44388</v>
       </c>
       <c r="C123" t="inlineStr"/>
       <c r="D123" t="inlineStr">
@@ -3153,10 +2913,8 @@
       <c r="A124" t="n">
         <v>6420210711</v>
       </c>
-      <c r="B124" t="inlineStr">
-        <is>
-          <t>2021-07-11</t>
-        </is>
+      <c r="B124" s="2" t="n">
+        <v>44388</v>
       </c>
       <c r="C124" t="inlineStr"/>
       <c r="D124" t="inlineStr">
@@ -3175,10 +2933,8 @@
       <c r="A125" t="n">
         <v>6420210711</v>
       </c>
-      <c r="B125" t="inlineStr">
-        <is>
-          <t>2021-07-11</t>
-        </is>
+      <c r="B125" s="2" t="n">
+        <v>44388</v>
       </c>
       <c r="C125" t="inlineStr"/>
       <c r="D125" t="inlineStr">
@@ -3197,10 +2953,8 @@
       <c r="A126" t="n">
         <v>6520210711</v>
       </c>
-      <c r="B126" t="inlineStr">
-        <is>
-          <t>2021-07-11</t>
-        </is>
+      <c r="B126" s="2" t="n">
+        <v>44388</v>
       </c>
       <c r="C126" t="inlineStr"/>
       <c r="D126" t="inlineStr">
@@ -3219,10 +2973,8 @@
       <c r="A127" t="n">
         <v>6620210711</v>
       </c>
-      <c r="B127" t="inlineStr">
-        <is>
-          <t>2021-07-11</t>
-        </is>
+      <c r="B127" s="2" t="n">
+        <v>44388</v>
       </c>
       <c r="C127" t="inlineStr"/>
       <c r="D127" t="inlineStr">
@@ -3241,10 +2993,8 @@
       <c r="A128" t="n">
         <v>6620210712</v>
       </c>
-      <c r="B128" t="inlineStr">
-        <is>
-          <t>2021-07-12</t>
-        </is>
+      <c r="B128" s="2" t="n">
+        <v>44389</v>
       </c>
       <c r="C128" t="inlineStr"/>
       <c r="D128" t="inlineStr">
@@ -3263,10 +3013,8 @@
       <c r="A129" t="n">
         <v>6620210712</v>
       </c>
-      <c r="B129" t="inlineStr">
-        <is>
-          <t>2021-07-12</t>
-        </is>
+      <c r="B129" s="2" t="n">
+        <v>44389</v>
       </c>
       <c r="C129" t="inlineStr"/>
       <c r="D129" t="inlineStr">
@@ -3285,10 +3033,8 @@
       <c r="A130" t="n">
         <v>6720210712</v>
       </c>
-      <c r="B130" t="inlineStr">
-        <is>
-          <t>2021-07-12</t>
-        </is>
+      <c r="B130" s="2" t="n">
+        <v>44389</v>
       </c>
       <c r="C130" t="inlineStr"/>
       <c r="D130" t="inlineStr">
@@ -3307,10 +3053,8 @@
       <c r="A131" t="n">
         <v>6820210713</v>
       </c>
-      <c r="B131" t="inlineStr">
-        <is>
-          <t>2021-07-13</t>
-        </is>
+      <c r="B131" s="2" t="n">
+        <v>44390</v>
       </c>
       <c r="C131" t="inlineStr"/>
       <c r="D131" t="inlineStr">
@@ -3329,10 +3073,8 @@
       <c r="A132" t="n">
         <v>6920210713</v>
       </c>
-      <c r="B132" t="inlineStr">
-        <is>
-          <t>2021-07-13</t>
-        </is>
+      <c r="B132" s="2" t="n">
+        <v>44390</v>
       </c>
       <c r="C132" t="inlineStr"/>
       <c r="D132" t="inlineStr">
@@ -3351,10 +3093,8 @@
       <c r="A133" t="n">
         <v>7020210714</v>
       </c>
-      <c r="B133" t="inlineStr">
-        <is>
-          <t>2021-07-14</t>
-        </is>
+      <c r="B133" s="2" t="n">
+        <v>44391</v>
       </c>
       <c r="C133" t="inlineStr"/>
       <c r="D133" t="inlineStr">
@@ -3373,10 +3113,8 @@
       <c r="A134" t="n">
         <v>7020210714</v>
       </c>
-      <c r="B134" t="inlineStr">
-        <is>
-          <t>2021-07-14</t>
-        </is>
+      <c r="B134" s="2" t="n">
+        <v>44391</v>
       </c>
       <c r="C134" t="inlineStr"/>
       <c r="D134" t="inlineStr">
@@ -3395,10 +3133,8 @@
       <c r="A135" t="n">
         <v>7020210714</v>
       </c>
-      <c r="B135" t="inlineStr">
-        <is>
-          <t>2021-07-14</t>
-        </is>
+      <c r="B135" s="2" t="n">
+        <v>44391</v>
       </c>
       <c r="C135" t="inlineStr"/>
       <c r="D135" t="inlineStr">
@@ -3417,10 +3153,8 @@
       <c r="A136" t="n">
         <v>7020210715</v>
       </c>
-      <c r="B136" t="inlineStr">
-        <is>
-          <t>2021-07-15</t>
-        </is>
+      <c r="B136" s="2" t="n">
+        <v>44392</v>
       </c>
       <c r="C136" t="inlineStr"/>
       <c r="D136" t="inlineStr">
@@ -3439,10 +3173,8 @@
       <c r="A137" t="n">
         <v>7020210715</v>
       </c>
-      <c r="B137" t="inlineStr">
-        <is>
-          <t>2021-07-15</t>
-        </is>
+      <c r="B137" s="2" t="n">
+        <v>44392</v>
       </c>
       <c r="C137" t="inlineStr"/>
       <c r="D137" t="inlineStr">
@@ -3461,10 +3193,8 @@
       <c r="A138" t="n">
         <v>7020210715</v>
       </c>
-      <c r="B138" t="inlineStr">
-        <is>
-          <t>2021-07-15</t>
-        </is>
+      <c r="B138" s="2" t="n">
+        <v>44392</v>
       </c>
       <c r="C138" t="inlineStr"/>
       <c r="D138" t="inlineStr">
@@ -3483,10 +3213,8 @@
       <c r="A139" t="n">
         <v>7120210716</v>
       </c>
-      <c r="B139" t="inlineStr">
-        <is>
-          <t>2021-07-16</t>
-        </is>
+      <c r="B139" s="2" t="n">
+        <v>44393</v>
       </c>
       <c r="C139" t="inlineStr"/>
       <c r="D139" t="inlineStr">
@@ -3505,10 +3233,8 @@
       <c r="A140" t="n">
         <v>7220210716</v>
       </c>
-      <c r="B140" t="inlineStr">
-        <is>
-          <t>2021-07-16</t>
-        </is>
+      <c r="B140" s="2" t="n">
+        <v>44393</v>
       </c>
       <c r="C140" t="inlineStr"/>
       <c r="D140" t="inlineStr">
@@ -3527,10 +3253,8 @@
       <c r="A141" t="n">
         <v>7320210716</v>
       </c>
-      <c r="B141" t="inlineStr">
-        <is>
-          <t>2021-07-16</t>
-        </is>
+      <c r="B141" s="2" t="n">
+        <v>44393</v>
       </c>
       <c r="C141" t="inlineStr"/>
       <c r="D141" t="inlineStr">
@@ -3549,10 +3273,8 @@
       <c r="A142" t="n">
         <v>7420210717</v>
       </c>
-      <c r="B142" t="inlineStr">
-        <is>
-          <t>2021-07-17</t>
-        </is>
+      <c r="B142" s="2" t="n">
+        <v>44394</v>
       </c>
       <c r="C142" t="inlineStr"/>
       <c r="D142" t="inlineStr">
@@ -3571,10 +3293,8 @@
       <c r="A143" t="n">
         <v>7520210717</v>
       </c>
-      <c r="B143" t="inlineStr">
-        <is>
-          <t>2021-07-17</t>
-        </is>
+      <c r="B143" s="2" t="n">
+        <v>44394</v>
       </c>
       <c r="C143" t="inlineStr"/>
       <c r="D143" t="inlineStr">
@@ -3593,10 +3313,8 @@
       <c r="A144" t="n">
         <v>7520210717</v>
       </c>
-      <c r="B144" t="inlineStr">
-        <is>
-          <t>2021-07-17</t>
-        </is>
+      <c r="B144" s="2" t="n">
+        <v>44394</v>
       </c>
       <c r="C144" t="inlineStr"/>
       <c r="D144" t="inlineStr">
@@ -3615,10 +3333,8 @@
       <c r="A145" t="n">
         <v>7620210717</v>
       </c>
-      <c r="B145" t="inlineStr">
-        <is>
-          <t>2021-07-17</t>
-        </is>
+      <c r="B145" s="2" t="n">
+        <v>44394</v>
       </c>
       <c r="C145" t="inlineStr"/>
       <c r="D145" t="inlineStr">
@@ -3637,10 +3353,8 @@
       <c r="A146" t="n">
         <v>7620210717</v>
       </c>
-      <c r="B146" t="inlineStr">
-        <is>
-          <t>2021-07-17</t>
-        </is>
+      <c r="B146" s="2" t="n">
+        <v>44394</v>
       </c>
       <c r="C146" t="inlineStr"/>
       <c r="D146" t="inlineStr">
@@ -3659,10 +3373,8 @@
       <c r="A147" t="n">
         <v>7720210717</v>
       </c>
-      <c r="B147" t="inlineStr">
-        <is>
-          <t>2021-07-17</t>
-        </is>
+      <c r="B147" s="2" t="n">
+        <v>44394</v>
       </c>
       <c r="C147" t="inlineStr"/>
       <c r="D147" t="inlineStr">
@@ -3681,10 +3393,8 @@
       <c r="A148" t="n">
         <v>7820210718</v>
       </c>
-      <c r="B148" t="inlineStr">
-        <is>
-          <t>2021-07-18</t>
-        </is>
+      <c r="B148" s="2" t="n">
+        <v>44395</v>
       </c>
       <c r="C148" t="inlineStr"/>
       <c r="D148" t="inlineStr">
@@ -3703,10 +3413,8 @@
       <c r="A149" t="n">
         <v>7920210718</v>
       </c>
-      <c r="B149" t="inlineStr">
-        <is>
-          <t>2021-07-18</t>
-        </is>
+      <c r="B149" s="2" t="n">
+        <v>44395</v>
       </c>
       <c r="C149" t="inlineStr"/>
       <c r="D149" t="inlineStr">
@@ -3725,10 +3433,8 @@
       <c r="A150" t="n">
         <v>8020210718</v>
       </c>
-      <c r="B150" t="inlineStr">
-        <is>
-          <t>2021-07-18</t>
-        </is>
+      <c r="B150" s="2" t="n">
+        <v>44395</v>
       </c>
       <c r="C150" t="inlineStr"/>
       <c r="D150" t="inlineStr">
@@ -3747,10 +3453,8 @@
       <c r="A151" t="n">
         <v>8020210718</v>
       </c>
-      <c r="B151" t="inlineStr">
-        <is>
-          <t>2021-07-18</t>
-        </is>
+      <c r="B151" s="2" t="n">
+        <v>44395</v>
       </c>
       <c r="C151" t="inlineStr"/>
       <c r="D151" t="inlineStr">
@@ -3769,10 +3473,8 @@
       <c r="A152" t="n">
         <v>8020210718</v>
       </c>
-      <c r="B152" t="inlineStr">
-        <is>
-          <t>2021-07-18</t>
-        </is>
+      <c r="B152" s="2" t="n">
+        <v>44395</v>
       </c>
       <c r="C152" t="inlineStr"/>
       <c r="D152" t="inlineStr">
@@ -3791,10 +3493,8 @@
       <c r="A153" t="n">
         <v>8120210718</v>
       </c>
-      <c r="B153" t="inlineStr">
-        <is>
-          <t>2021-07-18</t>
-        </is>
+      <c r="B153" s="2" t="n">
+        <v>44395</v>
       </c>
       <c r="C153" t="inlineStr"/>
       <c r="D153" t="inlineStr">
@@ -3813,10 +3513,8 @@
       <c r="A154" t="n">
         <v>8120210719</v>
       </c>
-      <c r="B154" t="inlineStr">
-        <is>
-          <t>2021-07-19</t>
-        </is>
+      <c r="B154" s="2" t="n">
+        <v>44396</v>
       </c>
       <c r="C154" t="inlineStr"/>
       <c r="D154" t="inlineStr">
@@ -3835,10 +3533,8 @@
       <c r="A155" t="n">
         <v>8220210719</v>
       </c>
-      <c r="B155" t="inlineStr">
-        <is>
-          <t>2021-07-19</t>
-        </is>
+      <c r="B155" s="2" t="n">
+        <v>44396</v>
       </c>
       <c r="C155" t="inlineStr"/>
       <c r="D155" t="inlineStr">
@@ -3857,10 +3553,8 @@
       <c r="A156" t="n">
         <v>8320210720</v>
       </c>
-      <c r="B156" t="inlineStr">
-        <is>
-          <t>2021-07-20</t>
-        </is>
+      <c r="B156" s="2" t="n">
+        <v>44397</v>
       </c>
       <c r="C156" t="inlineStr"/>
       <c r="D156" t="inlineStr">
@@ -3879,10 +3573,8 @@
       <c r="A157" t="n">
         <v>8320210720</v>
       </c>
-      <c r="B157" t="inlineStr">
-        <is>
-          <t>2021-07-20</t>
-        </is>
+      <c r="B157" s="2" t="n">
+        <v>44397</v>
       </c>
       <c r="C157" t="inlineStr"/>
       <c r="D157" t="inlineStr">
@@ -3901,10 +3593,8 @@
       <c r="A158" t="n">
         <v>8320210720</v>
       </c>
-      <c r="B158" t="inlineStr">
-        <is>
-          <t>2021-07-20</t>
-        </is>
+      <c r="B158" s="2" t="n">
+        <v>44397</v>
       </c>
       <c r="C158" t="inlineStr"/>
       <c r="D158" t="inlineStr">
@@ -3923,10 +3613,8 @@
       <c r="A159" t="n">
         <v>8420210721</v>
       </c>
-      <c r="B159" t="inlineStr">
-        <is>
-          <t>2021-07-21</t>
-        </is>
+      <c r="B159" s="2" t="n">
+        <v>44398</v>
       </c>
       <c r="C159" t="inlineStr"/>
       <c r="D159" t="inlineStr">
@@ -3945,10 +3633,8 @@
       <c r="A160" t="n">
         <v>8520210721</v>
       </c>
-      <c r="B160" t="inlineStr">
-        <is>
-          <t>2021-07-21</t>
-        </is>
+      <c r="B160" s="2" t="n">
+        <v>44398</v>
       </c>
       <c r="C160" t="inlineStr"/>
       <c r="D160" t="inlineStr">
@@ -3967,10 +3653,8 @@
       <c r="A161" t="n">
         <v>8620210722</v>
       </c>
-      <c r="B161" t="inlineStr">
-        <is>
-          <t>2021-07-22</t>
-        </is>
+      <c r="B161" s="2" t="n">
+        <v>44399</v>
       </c>
       <c r="C161" t="inlineStr"/>
       <c r="D161" t="inlineStr">
@@ -3989,10 +3673,8 @@
       <c r="A162" t="n">
         <v>8620210722</v>
       </c>
-      <c r="B162" t="inlineStr">
-        <is>
-          <t>2021-07-22</t>
-        </is>
+      <c r="B162" s="2" t="n">
+        <v>44399</v>
       </c>
       <c r="C162" t="inlineStr"/>
       <c r="D162" t="inlineStr">
@@ -4011,10 +3693,8 @@
       <c r="A163" t="n">
         <v>8620210722</v>
       </c>
-      <c r="B163" t="inlineStr">
-        <is>
-          <t>2021-07-22</t>
-        </is>
+      <c r="B163" s="2" t="n">
+        <v>44399</v>
       </c>
       <c r="C163" t="inlineStr"/>
       <c r="D163" t="inlineStr">
@@ -4033,10 +3713,8 @@
       <c r="A164" t="n">
         <v>8620210723</v>
       </c>
-      <c r="B164" t="inlineStr">
-        <is>
-          <t>2021-07-23</t>
-        </is>
+      <c r="B164" s="2" t="n">
+        <v>44400</v>
       </c>
       <c r="C164" t="inlineStr"/>
       <c r="D164" t="inlineStr">
@@ -4055,10 +3733,8 @@
       <c r="A165" t="n">
         <v>8620210723</v>
       </c>
-      <c r="B165" t="inlineStr">
-        <is>
-          <t>2021-07-23</t>
-        </is>
+      <c r="B165" s="2" t="n">
+        <v>44400</v>
       </c>
       <c r="C165" t="inlineStr"/>
       <c r="D165" t="inlineStr">
@@ -4077,10 +3753,8 @@
       <c r="A166" t="n">
         <v>8620210723</v>
       </c>
-      <c r="B166" t="inlineStr">
-        <is>
-          <t>2021-07-23</t>
-        </is>
+      <c r="B166" s="2" t="n">
+        <v>44400</v>
       </c>
       <c r="C166" t="inlineStr"/>
       <c r="D166" t="inlineStr">
@@ -4099,10 +3773,8 @@
       <c r="A167" t="n">
         <v>8620210723</v>
       </c>
-      <c r="B167" t="inlineStr">
-        <is>
-          <t>2021-07-23</t>
-        </is>
+      <c r="B167" s="2" t="n">
+        <v>44400</v>
       </c>
       <c r="C167" t="inlineStr"/>
       <c r="D167" t="inlineStr">
@@ -4121,10 +3793,8 @@
       <c r="A168" t="n">
         <v>8620210723</v>
       </c>
-      <c r="B168" t="inlineStr">
-        <is>
-          <t>2021-07-23</t>
-        </is>
+      <c r="B168" s="2" t="n">
+        <v>44400</v>
       </c>
       <c r="C168" t="inlineStr"/>
       <c r="D168" t="inlineStr">
@@ -4143,10 +3813,8 @@
       <c r="A169" t="n">
         <v>8720210723</v>
       </c>
-      <c r="B169" t="inlineStr">
-        <is>
-          <t>2021-07-23</t>
-        </is>
+      <c r="B169" s="2" t="n">
+        <v>44400</v>
       </c>
       <c r="C169" t="inlineStr"/>
       <c r="D169" t="inlineStr">
@@ -4165,10 +3833,8 @@
       <c r="A170" t="n">
         <v>8720210724</v>
       </c>
-      <c r="B170" t="inlineStr">
-        <is>
-          <t>2021-07-24</t>
-        </is>
+      <c r="B170" s="2" t="n">
+        <v>44401</v>
       </c>
       <c r="C170" t="inlineStr"/>
       <c r="D170" t="inlineStr">
@@ -4187,10 +3853,8 @@
       <c r="A171" t="n">
         <v>8820210724</v>
       </c>
-      <c r="B171" t="inlineStr">
-        <is>
-          <t>2021-07-24</t>
-        </is>
+      <c r="B171" s="2" t="n">
+        <v>44401</v>
       </c>
       <c r="C171" t="inlineStr"/>
       <c r="D171" t="inlineStr">
@@ -4209,10 +3873,8 @@
       <c r="A172" t="n">
         <v>8920210724</v>
       </c>
-      <c r="B172" t="inlineStr">
-        <is>
-          <t>2021-07-24</t>
-        </is>
+      <c r="B172" s="2" t="n">
+        <v>44401</v>
       </c>
       <c r="C172" t="inlineStr"/>
       <c r="D172" t="inlineStr">
@@ -4231,10 +3893,8 @@
       <c r="A173" t="n">
         <v>8920210724</v>
       </c>
-      <c r="B173" t="inlineStr">
-        <is>
-          <t>2021-07-24</t>
-        </is>
+      <c r="B173" s="2" t="n">
+        <v>44401</v>
       </c>
       <c r="C173" t="inlineStr"/>
       <c r="D173" t="inlineStr">
@@ -4253,10 +3913,8 @@
       <c r="A174" t="n">
         <v>8920210724</v>
       </c>
-      <c r="B174" t="inlineStr">
-        <is>
-          <t>2021-07-24</t>
-        </is>
+      <c r="B174" s="2" t="n">
+        <v>44401</v>
       </c>
       <c r="C174" t="inlineStr"/>
       <c r="D174" t="inlineStr">
@@ -4275,10 +3933,8 @@
       <c r="A175" t="n">
         <v>9020210725</v>
       </c>
-      <c r="B175" t="inlineStr">
-        <is>
-          <t>2021-07-25</t>
-        </is>
+      <c r="B175" s="2" t="n">
+        <v>44402</v>
       </c>
       <c r="C175" t="inlineStr"/>
       <c r="D175" t="inlineStr">
@@ -4297,10 +3953,8 @@
       <c r="A176" t="n">
         <v>9020210725</v>
       </c>
-      <c r="B176" t="inlineStr">
-        <is>
-          <t>2021-07-25</t>
-        </is>
+      <c r="B176" s="2" t="n">
+        <v>44402</v>
       </c>
       <c r="C176" t="inlineStr"/>
       <c r="D176" t="inlineStr">
@@ -4319,10 +3973,8 @@
       <c r="A177" t="n">
         <v>9020210725</v>
       </c>
-      <c r="B177" t="inlineStr">
-        <is>
-          <t>2021-07-25</t>
-        </is>
+      <c r="B177" s="2" t="n">
+        <v>44402</v>
       </c>
       <c r="C177" t="inlineStr"/>
       <c r="D177" t="inlineStr">
@@ -4341,10 +3993,8 @@
       <c r="A178" t="n">
         <v>9120210725</v>
       </c>
-      <c r="B178" t="inlineStr">
-        <is>
-          <t>2021-07-25</t>
-        </is>
+      <c r="B178" s="2" t="n">
+        <v>44402</v>
       </c>
       <c r="C178" t="inlineStr"/>
       <c r="D178" t="inlineStr">
@@ -4363,10 +4013,8 @@
       <c r="A179" t="n">
         <v>9120210725</v>
       </c>
-      <c r="B179" t="inlineStr">
-        <is>
-          <t>2021-07-25</t>
-        </is>
+      <c r="B179" s="2" t="n">
+        <v>44402</v>
       </c>
       <c r="C179" t="inlineStr"/>
       <c r="D179" t="inlineStr">
@@ -4385,10 +4033,8 @@
       <c r="A180" t="n">
         <v>9220210726</v>
       </c>
-      <c r="B180" t="inlineStr">
-        <is>
-          <t>2021-07-26</t>
-        </is>
+      <c r="B180" s="2" t="n">
+        <v>44403</v>
       </c>
       <c r="C180" t="inlineStr"/>
       <c r="D180" t="inlineStr">
@@ -4407,10 +4053,8 @@
       <c r="A181" t="n">
         <v>9220210726</v>
       </c>
-      <c r="B181" t="inlineStr">
-        <is>
-          <t>2021-07-26</t>
-        </is>
+      <c r="B181" s="2" t="n">
+        <v>44403</v>
       </c>
       <c r="C181" t="inlineStr"/>
       <c r="D181" t="inlineStr">
@@ -4429,10 +4073,8 @@
       <c r="A182" t="n">
         <v>9220210727</v>
       </c>
-      <c r="B182" t="inlineStr">
-        <is>
-          <t>2021-07-27</t>
-        </is>
+      <c r="B182" s="2" t="n">
+        <v>44404</v>
       </c>
       <c r="C182" t="inlineStr"/>
       <c r="D182" t="inlineStr">
@@ -4451,10 +4093,8 @@
       <c r="A183" t="n">
         <v>9320210727</v>
       </c>
-      <c r="B183" t="inlineStr">
-        <is>
-          <t>2021-07-27</t>
-        </is>
+      <c r="B183" s="2" t="n">
+        <v>44404</v>
       </c>
       <c r="C183" t="inlineStr"/>
       <c r="D183" t="inlineStr">
@@ -4473,10 +4113,8 @@
       <c r="A184" t="n">
         <v>9420210728</v>
       </c>
-      <c r="B184" t="inlineStr">
-        <is>
-          <t>2021-07-28</t>
-        </is>
+      <c r="B184" s="2" t="n">
+        <v>44405</v>
       </c>
       <c r="C184" t="inlineStr"/>
       <c r="D184" t="inlineStr">
@@ -4495,10 +4133,8 @@
       <c r="A185" t="n">
         <v>9520210728</v>
       </c>
-      <c r="B185" t="inlineStr">
-        <is>
-          <t>2021-07-28</t>
-        </is>
+      <c r="B185" s="2" t="n">
+        <v>44405</v>
       </c>
       <c r="C185" t="inlineStr"/>
       <c r="D185" t="inlineStr">
@@ -4517,10 +4153,8 @@
       <c r="A186" t="n">
         <v>9520210728</v>
       </c>
-      <c r="B186" t="inlineStr">
-        <is>
-          <t>2021-07-28</t>
-        </is>
+      <c r="B186" s="2" t="n">
+        <v>44405</v>
       </c>
       <c r="C186" t="inlineStr"/>
       <c r="D186" t="inlineStr">
@@ -4539,10 +4173,8 @@
       <c r="A187" t="n">
         <v>9620210729</v>
       </c>
-      <c r="B187" t="inlineStr">
-        <is>
-          <t>2021-07-29</t>
-        </is>
+      <c r="B187" s="2" t="n">
+        <v>44406</v>
       </c>
       <c r="C187" t="inlineStr"/>
       <c r="D187" t="inlineStr">
@@ -4561,10 +4193,8 @@
       <c r="A188" t="n">
         <v>9720210729</v>
       </c>
-      <c r="B188" t="inlineStr">
-        <is>
-          <t>2021-07-29</t>
-        </is>
+      <c r="B188" s="2" t="n">
+        <v>44406</v>
       </c>
       <c r="C188" t="inlineStr"/>
       <c r="D188" t="inlineStr">
@@ -4583,10 +4213,8 @@
       <c r="A189" t="n">
         <v>9720210729</v>
       </c>
-      <c r="B189" t="inlineStr">
-        <is>
-          <t>2021-07-29</t>
-        </is>
+      <c r="B189" s="2" t="n">
+        <v>44406</v>
       </c>
       <c r="C189" t="inlineStr"/>
       <c r="D189" t="inlineStr">
@@ -4605,10 +4233,8 @@
       <c r="A190" t="n">
         <v>9720210730</v>
       </c>
-      <c r="B190" t="inlineStr">
-        <is>
-          <t>2021-07-30</t>
-        </is>
+      <c r="B190" s="2" t="n">
+        <v>44407</v>
       </c>
       <c r="C190" t="inlineStr"/>
       <c r="D190" t="inlineStr">
@@ -4627,10 +4253,8 @@
       <c r="A191" t="n">
         <v>9820210730</v>
       </c>
-      <c r="B191" t="inlineStr">
-        <is>
-          <t>2021-07-30</t>
-        </is>
+      <c r="B191" s="2" t="n">
+        <v>44407</v>
       </c>
       <c r="C191" t="inlineStr"/>
       <c r="D191" t="inlineStr">
@@ -4649,10 +4273,8 @@
       <c r="A192" t="n">
         <v>9920210730</v>
       </c>
-      <c r="B192" t="inlineStr">
-        <is>
-          <t>2021-07-30</t>
-        </is>
+      <c r="B192" s="2" t="n">
+        <v>44407</v>
       </c>
       <c r="C192" t="inlineStr"/>
       <c r="D192" t="inlineStr">
@@ -4671,10 +4293,8 @@
       <c r="A193" t="n">
         <v>10020210731</v>
       </c>
-      <c r="B193" t="inlineStr">
-        <is>
-          <t>2021-07-31</t>
-        </is>
+      <c r="B193" s="2" t="n">
+        <v>44408</v>
       </c>
       <c r="C193" t="inlineStr"/>
       <c r="D193" t="inlineStr">
@@ -4693,10 +4313,8 @@
       <c r="A194" t="n">
         <v>10120210731</v>
       </c>
-      <c r="B194" t="inlineStr">
-        <is>
-          <t>2021-07-31</t>
-        </is>
+      <c r="B194" s="2" t="n">
+        <v>44408</v>
       </c>
       <c r="C194" t="inlineStr"/>
       <c r="D194" t="inlineStr">
@@ -4715,10 +4333,8 @@
       <c r="A195" t="n">
         <v>10120210731</v>
       </c>
-      <c r="B195" t="inlineStr">
-        <is>
-          <t>2021-07-31</t>
-        </is>
+      <c r="B195" s="2" t="n">
+        <v>44408</v>
       </c>
       <c r="C195" t="inlineStr"/>
       <c r="D195" t="inlineStr">
@@ -4737,10 +4353,8 @@
       <c r="A196" t="n">
         <v>10120210731</v>
       </c>
-      <c r="B196" t="inlineStr">
-        <is>
-          <t>2021-07-31</t>
-        </is>
+      <c r="B196" s="2" t="n">
+        <v>44408</v>
       </c>
       <c r="C196" t="inlineStr"/>
       <c r="D196" t="inlineStr">
@@ -4759,10 +4373,8 @@
       <c r="A197" t="n">
         <v>10120210731</v>
       </c>
-      <c r="B197" t="inlineStr">
-        <is>
-          <t>2021-07-31</t>
-        </is>
+      <c r="B197" s="2" t="n">
+        <v>44408</v>
       </c>
       <c r="C197" t="inlineStr"/>
       <c r="D197" t="inlineStr">
@@ -4781,10 +4393,8 @@
       <c r="A198" t="n">
         <v>10220210731</v>
       </c>
-      <c r="B198" t="inlineStr">
-        <is>
-          <t>2021-07-31</t>
-        </is>
+      <c r="B198" s="2" t="n">
+        <v>44408</v>
       </c>
       <c r="C198" t="inlineStr"/>
       <c r="D198" t="inlineStr">
@@ -4803,10 +4413,8 @@
       <c r="A199" t="n">
         <v>10220210801</v>
       </c>
-      <c r="B199" t="inlineStr">
-        <is>
-          <t>2021-08-01</t>
-        </is>
+      <c r="B199" s="2" t="n">
+        <v>44409</v>
       </c>
       <c r="C199" t="inlineStr"/>
       <c r="D199" t="inlineStr">
@@ -4825,10 +4433,8 @@
       <c r="A200" t="n">
         <v>10320210801</v>
       </c>
-      <c r="B200" t="inlineStr">
-        <is>
-          <t>2021-08-01</t>
-        </is>
+      <c r="B200" s="2" t="n">
+        <v>44409</v>
       </c>
       <c r="C200" t="inlineStr"/>
       <c r="D200" t="inlineStr">
@@ -4847,10 +4453,8 @@
       <c r="A201" t="n">
         <v>10320210801</v>
       </c>
-      <c r="B201" t="inlineStr">
-        <is>
-          <t>2021-08-01</t>
-        </is>
+      <c r="B201" s="2" t="n">
+        <v>44409</v>
       </c>
       <c r="C201" t="inlineStr"/>
       <c r="D201" t="inlineStr">
@@ -4869,10 +4473,8 @@
       <c r="A202" t="n">
         <v>10420210801</v>
       </c>
-      <c r="B202" t="inlineStr">
-        <is>
-          <t>2021-08-01</t>
-        </is>
+      <c r="B202" s="2" t="n">
+        <v>44409</v>
       </c>
       <c r="C202" t="inlineStr"/>
       <c r="D202" t="inlineStr">
@@ -4891,10 +4493,8 @@
       <c r="A203" t="n">
         <v>10420210801</v>
       </c>
-      <c r="B203" t="inlineStr">
-        <is>
-          <t>2021-08-01</t>
-        </is>
+      <c r="B203" s="2" t="n">
+        <v>44409</v>
       </c>
       <c r="C203" t="inlineStr"/>
       <c r="D203" t="inlineStr">
@@ -4913,10 +4513,8 @@
       <c r="A204" t="n">
         <v>10420210801</v>
       </c>
-      <c r="B204" t="inlineStr">
-        <is>
-          <t>2021-08-01</t>
-        </is>
+      <c r="B204" s="2" t="n">
+        <v>44409</v>
       </c>
       <c r="C204" t="inlineStr"/>
       <c r="D204" t="inlineStr">
@@ -4935,10 +4533,8 @@
       <c r="A205" t="n">
         <v>10420210805</v>
       </c>
-      <c r="B205" t="inlineStr">
-        <is>
-          <t>2021-08-05</t>
-        </is>
+      <c r="B205" s="2" t="n">
+        <v>44413</v>
       </c>
       <c r="C205" t="inlineStr"/>
       <c r="D205" t="inlineStr">
@@ -4957,10 +4553,8 @@
       <c r="A206" t="n">
         <v>10420210805</v>
       </c>
-      <c r="B206" t="inlineStr">
-        <is>
-          <t>2021-08-05</t>
-        </is>
+      <c r="B206" s="2" t="n">
+        <v>44413</v>
       </c>
       <c r="C206" t="inlineStr"/>
       <c r="D206" t="inlineStr">
@@ -4979,10 +4573,8 @@
       <c r="A207" t="n">
         <v>10520210805</v>
       </c>
-      <c r="B207" t="inlineStr">
-        <is>
-          <t>2021-08-05</t>
-        </is>
+      <c r="B207" s="2" t="n">
+        <v>44413</v>
       </c>
       <c r="C207" t="inlineStr"/>
       <c r="D207" t="inlineStr">
@@ -5001,10 +4593,8 @@
       <c r="A208" t="n">
         <v>10520210806</v>
       </c>
-      <c r="B208" t="inlineStr">
-        <is>
-          <t>2021-08-06</t>
-        </is>
+      <c r="B208" s="2" t="n">
+        <v>44414</v>
       </c>
       <c r="C208" t="inlineStr"/>
       <c r="D208" t="inlineStr">
@@ -5023,10 +4613,8 @@
       <c r="A209" t="n">
         <v>10520210806</v>
       </c>
-      <c r="B209" t="inlineStr">
-        <is>
-          <t>2021-08-06</t>
-        </is>
+      <c r="B209" s="2" t="n">
+        <v>44414</v>
       </c>
       <c r="C209" t="inlineStr"/>
       <c r="D209" t="inlineStr">
@@ -5045,10 +4633,8 @@
       <c r="A210" t="n">
         <v>10520210806</v>
       </c>
-      <c r="B210" t="inlineStr">
-        <is>
-          <t>2021-08-06</t>
-        </is>
+      <c r="B210" s="2" t="n">
+        <v>44414</v>
       </c>
       <c r="C210" t="inlineStr"/>
       <c r="D210" t="inlineStr">
@@ -5067,10 +4653,8 @@
       <c r="A211" t="n">
         <v>10520210806</v>
       </c>
-      <c r="B211" t="inlineStr">
-        <is>
-          <t>2021-08-06</t>
-        </is>
+      <c r="B211" s="2" t="n">
+        <v>44414</v>
       </c>
       <c r="C211" t="inlineStr"/>
       <c r="D211" t="inlineStr">
@@ -5089,10 +4673,8 @@
       <c r="A212" t="n">
         <v>10520210806</v>
       </c>
-      <c r="B212" t="inlineStr">
-        <is>
-          <t>2021-08-06</t>
-        </is>
+      <c r="B212" s="2" t="n">
+        <v>44414</v>
       </c>
       <c r="C212" t="inlineStr"/>
       <c r="D212" t="inlineStr">
@@ -5111,10 +4693,8 @@
       <c r="A213" t="n">
         <v>10620210806</v>
       </c>
-      <c r="B213" t="inlineStr">
-        <is>
-          <t>2021-08-06</t>
-        </is>
+      <c r="B213" s="2" t="n">
+        <v>44414</v>
       </c>
       <c r="C213" t="inlineStr"/>
       <c r="D213" t="inlineStr">
@@ -5133,10 +4713,8 @@
       <c r="A214" t="n">
         <v>10720210807</v>
       </c>
-      <c r="B214" t="inlineStr">
-        <is>
-          <t>2021-08-07</t>
-        </is>
+      <c r="B214" s="2" t="n">
+        <v>44415</v>
       </c>
       <c r="C214" t="inlineStr"/>
       <c r="D214" t="inlineStr">
@@ -5155,10 +4733,8 @@
       <c r="A215" t="n">
         <v>10820210807</v>
       </c>
-      <c r="B215" t="inlineStr">
-        <is>
-          <t>2021-08-07</t>
-        </is>
+      <c r="B215" s="2" t="n">
+        <v>44415</v>
       </c>
       <c r="C215" t="inlineStr"/>
       <c r="D215" t="inlineStr">
@@ -5177,10 +4753,8 @@
       <c r="A216" t="n">
         <v>10820210807</v>
       </c>
-      <c r="B216" t="inlineStr">
-        <is>
-          <t>2021-08-07</t>
-        </is>
+      <c r="B216" s="2" t="n">
+        <v>44415</v>
       </c>
       <c r="C216" t="inlineStr"/>
       <c r="D216" t="inlineStr">
@@ -5199,10 +4773,8 @@
       <c r="A217" t="n">
         <v>10920210807</v>
       </c>
-      <c r="B217" t="inlineStr">
-        <is>
-          <t>2021-08-07</t>
-        </is>
+      <c r="B217" s="2" t="n">
+        <v>44415</v>
       </c>
       <c r="C217" t="inlineStr"/>
       <c r="D217" t="inlineStr">
@@ -5221,10 +4793,8 @@
       <c r="A218" t="n">
         <v>10920210807</v>
       </c>
-      <c r="B218" t="inlineStr">
-        <is>
-          <t>2021-08-07</t>
-        </is>
+      <c r="B218" s="2" t="n">
+        <v>44415</v>
       </c>
       <c r="C218" t="inlineStr"/>
       <c r="D218" t="inlineStr">
@@ -5243,10 +4813,8 @@
       <c r="A219" t="n">
         <v>10920210808</v>
       </c>
-      <c r="B219" t="inlineStr">
-        <is>
-          <t>2021-08-08</t>
-        </is>
+      <c r="B219" s="2" t="n">
+        <v>44416</v>
       </c>
       <c r="C219" t="inlineStr"/>
       <c r="D219" t="inlineStr">
@@ -5265,10 +4833,8 @@
       <c r="A220" t="n">
         <v>11020210808</v>
       </c>
-      <c r="B220" t="inlineStr">
-        <is>
-          <t>2021-08-08</t>
-        </is>
+      <c r="B220" s="2" t="n">
+        <v>44416</v>
       </c>
       <c r="C220" t="inlineStr"/>
       <c r="D220" t="inlineStr">
@@ -5287,10 +4853,8 @@
       <c r="A221" t="n">
         <v>11120210808</v>
       </c>
-      <c r="B221" t="inlineStr">
-        <is>
-          <t>2021-08-08</t>
-        </is>
+      <c r="B221" s="2" t="n">
+        <v>44416</v>
       </c>
       <c r="C221" t="inlineStr"/>
       <c r="D221" t="inlineStr">
@@ -5309,10 +4873,8 @@
       <c r="A222" t="n">
         <v>11220210808</v>
       </c>
-      <c r="B222" t="inlineStr">
-        <is>
-          <t>2021-08-08</t>
-        </is>
+      <c r="B222" s="2" t="n">
+        <v>44416</v>
       </c>
       <c r="C222" t="inlineStr"/>
       <c r="D222" t="inlineStr">
@@ -5331,10 +4893,8 @@
       <c r="A223" t="n">
         <v>11220210808</v>
       </c>
-      <c r="B223" t="inlineStr">
-        <is>
-          <t>2021-08-08</t>
-        </is>
+      <c r="B223" s="2" t="n">
+        <v>44416</v>
       </c>
       <c r="C223" t="inlineStr"/>
       <c r="D223" t="inlineStr">
@@ -5353,10 +4913,8 @@
       <c r="A224" t="n">
         <v>11220210808</v>
       </c>
-      <c r="B224" t="inlineStr">
-        <is>
-          <t>2021-08-08</t>
-        </is>
+      <c r="B224" s="2" t="n">
+        <v>44416</v>
       </c>
       <c r="C224" t="inlineStr"/>
       <c r="D224" t="inlineStr">
@@ -5375,10 +4933,8 @@
       <c r="A225" t="n">
         <v>11320210810</v>
       </c>
-      <c r="B225" t="inlineStr">
-        <is>
-          <t>2021-08-10</t>
-        </is>
+      <c r="B225" s="2" t="n">
+        <v>44418</v>
       </c>
       <c r="C225" t="inlineStr"/>
       <c r="D225" t="inlineStr">
@@ -5397,10 +4953,8 @@
       <c r="A226" t="n">
         <v>11420210810</v>
       </c>
-      <c r="B226" t="inlineStr">
-        <is>
-          <t>2021-08-10</t>
-        </is>
+      <c r="B226" s="2" t="n">
+        <v>44418</v>
       </c>
       <c r="C226" t="inlineStr"/>
       <c r="D226" t="inlineStr">
@@ -5419,10 +4973,8 @@
       <c r="A227" t="n">
         <v>11520210812</v>
       </c>
-      <c r="B227" t="inlineStr">
-        <is>
-          <t>2021-08-12</t>
-        </is>
+      <c r="B227" s="2" t="n">
+        <v>44420</v>
       </c>
       <c r="C227" t="inlineStr"/>
       <c r="D227" t="inlineStr">
@@ -5441,10 +4993,8 @@
       <c r="A228" t="n">
         <v>11620210812</v>
       </c>
-      <c r="B228" t="inlineStr">
-        <is>
-          <t>2021-08-12</t>
-        </is>
+      <c r="B228" s="2" t="n">
+        <v>44420</v>
       </c>
       <c r="C228" t="inlineStr"/>
       <c r="D228" t="inlineStr">
@@ -5463,10 +5013,8 @@
       <c r="A229" t="n">
         <v>11620210812</v>
       </c>
-      <c r="B229" t="inlineStr">
-        <is>
-          <t>2021-08-12</t>
-        </is>
+      <c r="B229" s="2" t="n">
+        <v>44420</v>
       </c>
       <c r="C229" t="inlineStr"/>
       <c r="D229" t="inlineStr">
@@ -5485,10 +5033,8 @@
       <c r="A230" t="n">
         <v>11720210813</v>
       </c>
-      <c r="B230" t="inlineStr">
-        <is>
-          <t>2021-08-13</t>
-        </is>
+      <c r="B230" s="2" t="n">
+        <v>44421</v>
       </c>
       <c r="C230" t="inlineStr"/>
       <c r="D230" t="inlineStr">
@@ -5507,10 +5053,8 @@
       <c r="A231" t="n">
         <v>11720210813</v>
       </c>
-      <c r="B231" t="inlineStr">
-        <is>
-          <t>2021-08-13</t>
-        </is>
+      <c r="B231" s="2" t="n">
+        <v>44421</v>
       </c>
       <c r="C231" t="inlineStr"/>
       <c r="D231" t="inlineStr">
@@ -5529,10 +5073,8 @@
       <c r="A232" t="n">
         <v>11720210813</v>
       </c>
-      <c r="B232" t="inlineStr">
-        <is>
-          <t>2021-08-13</t>
-        </is>
+      <c r="B232" s="2" t="n">
+        <v>44421</v>
       </c>
       <c r="C232" t="inlineStr"/>
       <c r="D232" t="inlineStr">
@@ -5551,10 +5093,8 @@
       <c r="A233" t="n">
         <v>11820210813</v>
       </c>
-      <c r="B233" t="inlineStr">
-        <is>
-          <t>2021-08-13</t>
-        </is>
+      <c r="B233" s="2" t="n">
+        <v>44421</v>
       </c>
       <c r="C233" t="inlineStr"/>
       <c r="D233" t="inlineStr">
@@ -5573,10 +5113,8 @@
       <c r="A234" t="n">
         <v>11920210813</v>
       </c>
-      <c r="B234" t="inlineStr">
-        <is>
-          <t>2021-08-13</t>
-        </is>
+      <c r="B234" s="2" t="n">
+        <v>44421</v>
       </c>
       <c r="C234" t="inlineStr"/>
       <c r="D234" t="inlineStr">
@@ -5595,10 +5133,8 @@
       <c r="A235" t="n">
         <v>11920210813</v>
       </c>
-      <c r="B235" t="inlineStr">
-        <is>
-          <t>2021-08-13</t>
-        </is>
+      <c r="B235" s="2" t="n">
+        <v>44421</v>
       </c>
       <c r="C235" t="inlineStr"/>
       <c r="D235" t="inlineStr">
@@ -5617,10 +5153,8 @@
       <c r="A236" t="n">
         <v>12020210814</v>
       </c>
-      <c r="B236" t="inlineStr">
-        <is>
-          <t>2021-08-14</t>
-        </is>
+      <c r="B236" s="2" t="n">
+        <v>44422</v>
       </c>
       <c r="C236" t="inlineStr"/>
       <c r="D236" t="inlineStr">
@@ -5639,10 +5173,8 @@
       <c r="A237" t="n">
         <v>12120210814</v>
       </c>
-      <c r="B237" t="inlineStr">
-        <is>
-          <t>2021-08-14</t>
-        </is>
+      <c r="B237" s="2" t="n">
+        <v>44422</v>
       </c>
       <c r="C237" t="inlineStr"/>
       <c r="D237" t="inlineStr">
@@ -5661,10 +5193,8 @@
       <c r="A238" t="n">
         <v>12120210814</v>
       </c>
-      <c r="B238" t="inlineStr">
-        <is>
-          <t>2021-08-14</t>
-        </is>
+      <c r="B238" s="2" t="n">
+        <v>44422</v>
       </c>
       <c r="C238" t="inlineStr"/>
       <c r="D238" t="inlineStr">
@@ -5683,10 +5213,8 @@
       <c r="A239" t="n">
         <v>12220210814</v>
       </c>
-      <c r="B239" t="inlineStr">
-        <is>
-          <t>2021-08-14</t>
-        </is>
+      <c r="B239" s="2" t="n">
+        <v>44422</v>
       </c>
       <c r="C239" t="inlineStr"/>
       <c r="D239" t="inlineStr">
@@ -5705,10 +5233,8 @@
       <c r="A240" t="n">
         <v>12320210815</v>
       </c>
-      <c r="B240" t="inlineStr">
-        <is>
-          <t>2021-08-15</t>
-        </is>
+      <c r="B240" s="2" t="n">
+        <v>44423</v>
       </c>
       <c r="C240" t="inlineStr"/>
       <c r="D240" t="inlineStr">
@@ -5727,10 +5253,8 @@
       <c r="A241" t="n">
         <v>12420210815</v>
       </c>
-      <c r="B241" t="inlineStr">
-        <is>
-          <t>2021-08-15</t>
-        </is>
+      <c r="B241" s="2" t="n">
+        <v>44423</v>
       </c>
       <c r="C241" t="inlineStr"/>
       <c r="D241" t="inlineStr">
@@ -5749,10 +5273,8 @@
       <c r="A242" t="n">
         <v>12520210815</v>
       </c>
-      <c r="B242" t="inlineStr">
-        <is>
-          <t>2021-08-15</t>
-        </is>
+      <c r="B242" s="2" t="n">
+        <v>44423</v>
       </c>
       <c r="C242" t="inlineStr"/>
       <c r="D242" t="inlineStr">
@@ -5771,10 +5293,8 @@
       <c r="A243" t="n">
         <v>12620210815</v>
       </c>
-      <c r="B243" t="inlineStr">
-        <is>
-          <t>2021-08-15</t>
-        </is>
+      <c r="B243" s="2" t="n">
+        <v>44423</v>
       </c>
       <c r="C243" t="inlineStr"/>
       <c r="D243" t="inlineStr">
@@ -5793,10 +5313,8 @@
       <c r="A244" t="n">
         <v>12620210815</v>
       </c>
-      <c r="B244" t="inlineStr">
-        <is>
-          <t>2021-08-15</t>
-        </is>
+      <c r="B244" s="2" t="n">
+        <v>44423</v>
       </c>
       <c r="C244" t="inlineStr"/>
       <c r="D244" t="inlineStr">
@@ -5815,10 +5333,8 @@
       <c r="A245" t="n">
         <v>12720210815</v>
       </c>
-      <c r="B245" t="inlineStr">
-        <is>
-          <t>2021-08-15</t>
-        </is>
+      <c r="B245" s="2" t="n">
+        <v>44423</v>
       </c>
       <c r="C245" t="inlineStr"/>
       <c r="D245" t="inlineStr">
@@ -5837,10 +5353,8 @@
       <c r="A246" t="n">
         <v>12720210816</v>
       </c>
-      <c r="B246" t="inlineStr">
-        <is>
-          <t>2021-08-16</t>
-        </is>
+      <c r="B246" s="2" t="n">
+        <v>44424</v>
       </c>
       <c r="C246" t="inlineStr"/>
       <c r="D246" t="inlineStr">
@@ -5859,10 +5373,8 @@
       <c r="A247" t="n">
         <v>12720210816</v>
       </c>
-      <c r="B247" t="inlineStr">
-        <is>
-          <t>2021-08-16</t>
-        </is>
+      <c r="B247" s="2" t="n">
+        <v>44424</v>
       </c>
       <c r="C247" t="inlineStr"/>
       <c r="D247" t="inlineStr">
@@ -5881,10 +5393,8 @@
       <c r="A248" t="n">
         <v>12820210816</v>
       </c>
-      <c r="B248" t="inlineStr">
-        <is>
-          <t>2021-08-16</t>
-        </is>
+      <c r="B248" s="2" t="n">
+        <v>44424</v>
       </c>
       <c r="C248" t="inlineStr"/>
       <c r="D248" t="inlineStr">
@@ -5903,10 +5413,8 @@
       <c r="A249" t="n">
         <v>12820210817</v>
       </c>
-      <c r="B249" t="inlineStr">
-        <is>
-          <t>2021-08-17</t>
-        </is>
+      <c r="B249" s="2" t="n">
+        <v>44425</v>
       </c>
       <c r="C249" t="inlineStr"/>
       <c r="D249" t="inlineStr">
@@ -5925,10 +5433,8 @@
       <c r="A250" t="n">
         <v>12820210817</v>
       </c>
-      <c r="B250" t="inlineStr">
-        <is>
-          <t>2021-08-17</t>
-        </is>
+      <c r="B250" s="2" t="n">
+        <v>44425</v>
       </c>
       <c r="C250" t="inlineStr"/>
       <c r="D250" t="inlineStr">
@@ -5947,10 +5453,8 @@
       <c r="A251" t="n">
         <v>12920210818</v>
       </c>
-      <c r="B251" t="inlineStr">
-        <is>
-          <t>2021-08-18</t>
-        </is>
+      <c r="B251" s="2" t="n">
+        <v>44426</v>
       </c>
       <c r="C251" t="inlineStr"/>
       <c r="D251" t="inlineStr">
@@ -5969,10 +5473,8 @@
       <c r="A252" t="n">
         <v>13020210818</v>
       </c>
-      <c r="B252" t="inlineStr">
-        <is>
-          <t>2021-08-18</t>
-        </is>
+      <c r="B252" s="2" t="n">
+        <v>44426</v>
       </c>
       <c r="C252" t="inlineStr"/>
       <c r="D252" t="inlineStr">
@@ -5991,10 +5493,8 @@
       <c r="A253" t="n">
         <v>13020210819</v>
       </c>
-      <c r="B253" t="inlineStr">
-        <is>
-          <t>2021-08-19</t>
-        </is>
+      <c r="B253" s="2" t="n">
+        <v>44427</v>
       </c>
       <c r="C253" t="inlineStr"/>
       <c r="D253" t="inlineStr">
@@ -6013,10 +5513,8 @@
       <c r="A254" t="n">
         <v>13020210819</v>
       </c>
-      <c r="B254" t="inlineStr">
-        <is>
-          <t>2021-08-19</t>
-        </is>
+      <c r="B254" s="2" t="n">
+        <v>44427</v>
       </c>
       <c r="C254" t="inlineStr"/>
       <c r="D254" t="inlineStr">
@@ -6035,10 +5533,8 @@
       <c r="A255" t="n">
         <v>13120210820</v>
       </c>
-      <c r="B255" t="inlineStr">
-        <is>
-          <t>2021-08-20</t>
-        </is>
+      <c r="B255" s="2" t="n">
+        <v>44428</v>
       </c>
       <c r="C255" t="inlineStr"/>
       <c r="D255" t="inlineStr">
@@ -6057,10 +5553,8 @@
       <c r="A256" t="n">
         <v>13120210820</v>
       </c>
-      <c r="B256" t="inlineStr">
-        <is>
-          <t>2021-08-20</t>
-        </is>
+      <c r="B256" s="2" t="n">
+        <v>44428</v>
       </c>
       <c r="C256" t="inlineStr"/>
       <c r="D256" t="inlineStr">
@@ -6079,10 +5573,8 @@
       <c r="A257" t="n">
         <v>13120210820</v>
       </c>
-      <c r="B257" t="inlineStr">
-        <is>
-          <t>2021-08-20</t>
-        </is>
+      <c r="B257" s="2" t="n">
+        <v>44428</v>
       </c>
       <c r="C257" t="inlineStr"/>
       <c r="D257" t="inlineStr">
@@ -6101,10 +5593,8 @@
       <c r="A258" t="n">
         <v>13120210820</v>
       </c>
-      <c r="B258" t="inlineStr">
-        <is>
-          <t>2021-08-20</t>
-        </is>
+      <c r="B258" s="2" t="n">
+        <v>44428</v>
       </c>
       <c r="C258" t="inlineStr"/>
       <c r="D258" t="inlineStr">
@@ -6123,10 +5613,8 @@
       <c r="A259" t="n">
         <v>13220210821</v>
       </c>
-      <c r="B259" t="inlineStr">
-        <is>
-          <t>2021-08-21</t>
-        </is>
+      <c r="B259" s="2" t="n">
+        <v>44429</v>
       </c>
       <c r="C259" t="inlineStr"/>
       <c r="D259" t="inlineStr">
@@ -6145,10 +5633,8 @@
       <c r="A260" t="n">
         <v>13320210821</v>
       </c>
-      <c r="B260" t="inlineStr">
-        <is>
-          <t>2021-08-21</t>
-        </is>
+      <c r="B260" s="2" t="n">
+        <v>44429</v>
       </c>
       <c r="C260" t="inlineStr"/>
       <c r="D260" t="inlineStr">
@@ -6167,10 +5653,8 @@
       <c r="A261" t="n">
         <v>13320210821</v>
       </c>
-      <c r="B261" t="inlineStr">
-        <is>
-          <t>2021-08-21</t>
-        </is>
+      <c r="B261" s="2" t="n">
+        <v>44429</v>
       </c>
       <c r="C261" t="inlineStr"/>
       <c r="D261" t="inlineStr">
@@ -6189,10 +5673,8 @@
       <c r="A262" t="n">
         <v>13320210821</v>
       </c>
-      <c r="B262" t="inlineStr">
-        <is>
-          <t>2021-08-21</t>
-        </is>
+      <c r="B262" s="2" t="n">
+        <v>44429</v>
       </c>
       <c r="C262" t="inlineStr"/>
       <c r="D262" t="inlineStr">
@@ -6211,10 +5693,8 @@
       <c r="A263" t="n">
         <v>13420210822</v>
       </c>
-      <c r="B263" t="inlineStr">
-        <is>
-          <t>2021-08-22</t>
-        </is>
+      <c r="B263" s="2" t="n">
+        <v>44430</v>
       </c>
       <c r="C263" t="inlineStr"/>
       <c r="D263" t="inlineStr">
@@ -6233,10 +5713,8 @@
       <c r="A264" t="n">
         <v>13420210822</v>
       </c>
-      <c r="B264" t="inlineStr">
-        <is>
-          <t>2021-08-22</t>
-        </is>
+      <c r="B264" s="2" t="n">
+        <v>44430</v>
       </c>
       <c r="C264" t="inlineStr"/>
       <c r="D264" t="inlineStr">
@@ -6255,10 +5733,8 @@
       <c r="A265" t="n">
         <v>13420210822</v>
       </c>
-      <c r="B265" t="inlineStr">
-        <is>
-          <t>2021-08-22</t>
-        </is>
+      <c r="B265" s="2" t="n">
+        <v>44430</v>
       </c>
       <c r="C265" t="inlineStr"/>
       <c r="D265" t="inlineStr">
@@ -6277,10 +5753,8 @@
       <c r="A266" t="n">
         <v>13420210822</v>
       </c>
-      <c r="B266" t="inlineStr">
-        <is>
-          <t>2021-08-22</t>
-        </is>
+      <c r="B266" s="2" t="n">
+        <v>44430</v>
       </c>
       <c r="C266" t="inlineStr"/>
       <c r="D266" t="inlineStr">
@@ -6299,10 +5773,8 @@
       <c r="A267" t="n">
         <v>13520210823</v>
       </c>
-      <c r="B267" t="inlineStr">
-        <is>
-          <t>2021-08-23</t>
-        </is>
+      <c r="B267" s="2" t="n">
+        <v>44431</v>
       </c>
       <c r="C267" t="inlineStr"/>
       <c r="D267" t="inlineStr">
@@ -6321,10 +5793,8 @@
       <c r="A268" t="n">
         <v>13520210823</v>
       </c>
-      <c r="B268" t="inlineStr">
-        <is>
-          <t>2021-08-23</t>
-        </is>
+      <c r="B268" s="2" t="n">
+        <v>44431</v>
       </c>
       <c r="C268" t="inlineStr"/>
       <c r="D268" t="inlineStr">
@@ -6343,10 +5813,8 @@
       <c r="A269" t="n">
         <v>13620210823</v>
       </c>
-      <c r="B269" t="inlineStr">
-        <is>
-          <t>2021-08-23</t>
-        </is>
+      <c r="B269" s="2" t="n">
+        <v>44431</v>
       </c>
       <c r="C269" t="inlineStr"/>
       <c r="D269" t="inlineStr">
@@ -6365,10 +5833,8 @@
       <c r="A270" t="n">
         <v>13720210824</v>
       </c>
-      <c r="B270" t="inlineStr">
-        <is>
-          <t>2021-08-24</t>
-        </is>
+      <c r="B270" s="2" t="n">
+        <v>44432</v>
       </c>
       <c r="C270" t="inlineStr"/>
       <c r="D270" t="inlineStr">
@@ -6387,10 +5853,8 @@
       <c r="A271" t="n">
         <v>13820210824</v>
       </c>
-      <c r="B271" t="inlineStr">
-        <is>
-          <t>2021-08-24</t>
-        </is>
+      <c r="B271" s="2" t="n">
+        <v>44432</v>
       </c>
       <c r="C271" t="inlineStr"/>
       <c r="D271" t="inlineStr">
@@ -6409,10 +5873,8 @@
       <c r="A272" t="n">
         <v>13820210824</v>
       </c>
-      <c r="B272" t="inlineStr">
-        <is>
-          <t>2021-08-24</t>
-        </is>
+      <c r="B272" s="2" t="n">
+        <v>44432</v>
       </c>
       <c r="C272" t="inlineStr"/>
       <c r="D272" t="inlineStr">
@@ -6431,10 +5893,8 @@
       <c r="A273" t="n">
         <v>13820210825</v>
       </c>
-      <c r="B273" t="inlineStr">
-        <is>
-          <t>2021-08-25</t>
-        </is>
+      <c r="B273" s="2" t="n">
+        <v>44433</v>
       </c>
       <c r="C273" t="inlineStr"/>
       <c r="D273" t="inlineStr">
@@ -6453,10 +5913,8 @@
       <c r="A274" t="n">
         <v>13920210825</v>
       </c>
-      <c r="B274" t="inlineStr">
-        <is>
-          <t>2021-08-25</t>
-        </is>
+      <c r="B274" s="2" t="n">
+        <v>44433</v>
       </c>
       <c r="C274" t="inlineStr"/>
       <c r="D274" t="inlineStr">
@@ -6475,10 +5933,8 @@
       <c r="A275" t="n">
         <v>14020210826</v>
       </c>
-      <c r="B275" t="inlineStr">
-        <is>
-          <t>2021-08-26</t>
-        </is>
+      <c r="B275" s="2" t="n">
+        <v>44434</v>
       </c>
       <c r="C275" t="inlineStr"/>
       <c r="D275" t="inlineStr">
@@ -6497,10 +5953,8 @@
       <c r="A276" t="n">
         <v>14020210826</v>
       </c>
-      <c r="B276" t="inlineStr">
-        <is>
-          <t>2021-08-26</t>
-        </is>
+      <c r="B276" s="2" t="n">
+        <v>44434</v>
       </c>
       <c r="C276" t="inlineStr"/>
       <c r="D276" t="inlineStr">
@@ -6519,10 +5973,8 @@
       <c r="A277" t="n">
         <v>14020210826</v>
       </c>
-      <c r="B277" t="inlineStr">
-        <is>
-          <t>2021-08-26</t>
-        </is>
+      <c r="B277" s="2" t="n">
+        <v>44434</v>
       </c>
       <c r="C277" t="inlineStr"/>
       <c r="D277" t="inlineStr">
@@ -6541,10 +5993,8 @@
       <c r="A278" t="n">
         <v>14120210827</v>
       </c>
-      <c r="B278" t="inlineStr">
-        <is>
-          <t>2021-08-27</t>
-        </is>
+      <c r="B278" s="2" t="n">
+        <v>44435</v>
       </c>
       <c r="C278" t="inlineStr"/>
       <c r="D278" t="inlineStr">
@@ -6563,10 +6013,8 @@
       <c r="A279" t="n">
         <v>14120210827</v>
       </c>
-      <c r="B279" t="inlineStr">
-        <is>
-          <t>2021-08-27</t>
-        </is>
+      <c r="B279" s="2" t="n">
+        <v>44435</v>
       </c>
       <c r="C279" t="inlineStr"/>
       <c r="D279" t="inlineStr">
@@ -6585,10 +6033,8 @@
       <c r="A280" t="n">
         <v>14120210827</v>
       </c>
-      <c r="B280" t="inlineStr">
-        <is>
-          <t>2021-08-27</t>
-        </is>
+      <c r="B280" s="2" t="n">
+        <v>44435</v>
       </c>
       <c r="C280" t="inlineStr"/>
       <c r="D280" t="inlineStr">
@@ -6607,10 +6053,8 @@
       <c r="A281" t="n">
         <v>14220210828</v>
       </c>
-      <c r="B281" t="inlineStr">
-        <is>
-          <t>2021-08-28</t>
-        </is>
+      <c r="B281" s="2" t="n">
+        <v>44436</v>
       </c>
       <c r="C281" t="inlineStr"/>
       <c r="D281" t="inlineStr">
@@ -6629,10 +6073,8 @@
       <c r="A282" t="n">
         <v>14320210828</v>
       </c>
-      <c r="B282" t="inlineStr">
-        <is>
-          <t>2021-08-28</t>
-        </is>
+      <c r="B282" s="2" t="n">
+        <v>44436</v>
       </c>
       <c r="C282" t="inlineStr"/>
       <c r="D282" t="inlineStr">
@@ -6651,10 +6093,8 @@
       <c r="A283" t="n">
         <v>14320210828</v>
       </c>
-      <c r="B283" t="inlineStr">
-        <is>
-          <t>2021-08-28</t>
-        </is>
+      <c r="B283" s="2" t="n">
+        <v>44436</v>
       </c>
       <c r="C283" t="inlineStr"/>
       <c r="D283" t="inlineStr">
@@ -6673,10 +6113,8 @@
       <c r="A284" t="n">
         <v>14320210829</v>
       </c>
-      <c r="B284" t="inlineStr">
-        <is>
-          <t>2021-08-29</t>
-        </is>
+      <c r="B284" s="2" t="n">
+        <v>44437</v>
       </c>
       <c r="C284" t="inlineStr"/>
       <c r="D284" t="inlineStr">
@@ -6695,10 +6133,8 @@
       <c r="A285" t="n">
         <v>14320210829</v>
       </c>
-      <c r="B285" t="inlineStr">
-        <is>
-          <t>2021-08-29</t>
-        </is>
+      <c r="B285" s="2" t="n">
+        <v>44437</v>
       </c>
       <c r="C285" t="inlineStr"/>
       <c r="D285" t="inlineStr">
@@ -6717,10 +6153,8 @@
       <c r="A286" t="n">
         <v>14320210829</v>
       </c>
-      <c r="B286" t="inlineStr">
-        <is>
-          <t>2021-08-29</t>
-        </is>
+      <c r="B286" s="2" t="n">
+        <v>44437</v>
       </c>
       <c r="C286" t="inlineStr"/>
       <c r="D286" t="inlineStr">
@@ -6739,10 +6173,8 @@
       <c r="A287" t="n">
         <v>14420210829</v>
       </c>
-      <c r="B287" t="inlineStr">
-        <is>
-          <t>2021-08-29</t>
-        </is>
+      <c r="B287" s="2" t="n">
+        <v>44437</v>
       </c>
       <c r="C287" t="inlineStr"/>
       <c r="D287" t="inlineStr">
@@ -6761,10 +6193,8 @@
       <c r="A288" t="n">
         <v>14420210829</v>
       </c>
-      <c r="B288" t="inlineStr">
-        <is>
-          <t>2021-08-29</t>
-        </is>
+      <c r="B288" s="2" t="n">
+        <v>44437</v>
       </c>
       <c r="C288" t="inlineStr"/>
       <c r="D288" t="inlineStr">
@@ -6783,10 +6213,8 @@
       <c r="A289" t="n">
         <v>14420210830</v>
       </c>
-      <c r="B289" t="inlineStr">
-        <is>
-          <t>2021-08-30</t>
-        </is>
+      <c r="B289" s="2" t="n">
+        <v>44438</v>
       </c>
       <c r="C289" t="inlineStr"/>
       <c r="D289" t="inlineStr">
@@ -6805,10 +6233,8 @@
       <c r="A290" t="n">
         <v>14520210830</v>
       </c>
-      <c r="B290" t="inlineStr">
-        <is>
-          <t>2021-08-30</t>
-        </is>
+      <c r="B290" s="2" t="n">
+        <v>44438</v>
       </c>
       <c r="C290" t="inlineStr"/>
       <c r="D290" t="inlineStr">
@@ -6827,10 +6253,8 @@
       <c r="A291" t="n">
         <v>14520210831</v>
       </c>
-      <c r="B291" t="inlineStr">
-        <is>
-          <t>2021-08-31</t>
-        </is>
+      <c r="B291" s="2" t="n">
+        <v>44439</v>
       </c>
       <c r="C291" t="inlineStr"/>
       <c r="D291" t="inlineStr">
@@ -6849,10 +6273,8 @@
       <c r="A292" t="n">
         <v>14520210831</v>
       </c>
-      <c r="B292" t="inlineStr">
-        <is>
-          <t>2021-08-31</t>
-        </is>
+      <c r="B292" s="2" t="n">
+        <v>44439</v>
       </c>
       <c r="C292" t="inlineStr"/>
       <c r="D292" t="inlineStr">
@@ -6871,10 +6293,8 @@
       <c r="A293" t="n">
         <v>14520210831</v>
       </c>
-      <c r="B293" t="inlineStr">
-        <is>
-          <t>2021-08-31</t>
-        </is>
+      <c r="B293" s="2" t="n">
+        <v>44439</v>
       </c>
       <c r="C293" t="inlineStr"/>
       <c r="D293" t="inlineStr">
@@ -6893,10 +6313,8 @@
       <c r="A294" t="n">
         <v>14620210901</v>
       </c>
-      <c r="B294" t="inlineStr">
-        <is>
-          <t>2021-09-01</t>
-        </is>
+      <c r="B294" s="2" t="n">
+        <v>44440</v>
       </c>
       <c r="C294" t="inlineStr"/>
       <c r="D294" t="inlineStr">
@@ -6915,10 +6333,8 @@
       <c r="A295" t="n">
         <v>14720210901</v>
       </c>
-      <c r="B295" t="inlineStr">
-        <is>
-          <t>2021-09-01</t>
-        </is>
+      <c r="B295" s="2" t="n">
+        <v>44440</v>
       </c>
       <c r="C295" t="inlineStr"/>
       <c r="D295" t="inlineStr">
@@ -6937,10 +6353,8 @@
       <c r="A296" t="n">
         <v>14720210901</v>
       </c>
-      <c r="B296" t="inlineStr">
-        <is>
-          <t>2021-09-01</t>
-        </is>
+      <c r="B296" s="2" t="n">
+        <v>44440</v>
       </c>
       <c r="C296" t="inlineStr"/>
       <c r="D296" t="inlineStr">

</xml_diff>

<commit_message>
melhorando a variavel coeficiente de determinacao
</commit_message>
<xml_diff>
--- a/saida_final.xlsx
+++ b/saida_final.xlsx
@@ -476,7 +476,9 @@
       <c r="B2" s="2" t="n">
         <v>44348</v>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" t="n">
+        <v>80</v>
+      </c>
       <c r="D2" t="inlineStr">
         <is>
           <t>item C</t>
@@ -496,7 +498,9 @@
       <c r="B3" s="2" t="n">
         <v>44348</v>
       </c>
-      <c r="C3" t="inlineStr"/>
+      <c r="C3" t="n">
+        <v>30</v>
+      </c>
       <c r="D3" t="inlineStr">
         <is>
           <t>item A</t>
@@ -516,7 +520,9 @@
       <c r="B4" s="2" t="n">
         <v>44351</v>
       </c>
-      <c r="C4" t="inlineStr"/>
+      <c r="C4" t="n">
+        <v>20</v>
+      </c>
       <c r="D4" t="inlineStr">
         <is>
           <t>item C</t>
@@ -536,7 +542,9 @@
       <c r="B5" s="2" t="n">
         <v>44351</v>
       </c>
-      <c r="C5" t="inlineStr"/>
+      <c r="C5" t="n">
+        <v>60</v>
+      </c>
       <c r="D5" t="inlineStr">
         <is>
           <t>item B</t>
@@ -556,7 +564,9 @@
       <c r="B6" s="2" t="n">
         <v>44351</v>
       </c>
-      <c r="C6" t="inlineStr"/>
+      <c r="C6" t="n">
+        <v>40</v>
+      </c>
       <c r="D6" t="inlineStr">
         <is>
           <t>item C</t>
@@ -576,7 +586,9 @@
       <c r="B7" s="2" t="n">
         <v>44351</v>
       </c>
-      <c r="C7" t="inlineStr"/>
+      <c r="C7" t="n">
+        <v>30</v>
+      </c>
       <c r="D7" t="inlineStr">
         <is>
           <t>item B</t>
@@ -596,7 +608,9 @@
       <c r="B8" s="2" t="n">
         <v>44351</v>
       </c>
-      <c r="C8" t="inlineStr"/>
+      <c r="C8" t="n">
+        <v>25</v>
+      </c>
       <c r="D8" t="inlineStr">
         <is>
           <t>item D</t>
@@ -616,7 +630,9 @@
       <c r="B9" s="2" t="n">
         <v>44352</v>
       </c>
-      <c r="C9" t="inlineStr"/>
+      <c r="C9" t="n">
+        <v>25</v>
+      </c>
       <c r="D9" t="inlineStr">
         <is>
           <t>item D</t>
@@ -636,7 +652,9 @@
       <c r="B10" s="2" t="n">
         <v>44352</v>
       </c>
-      <c r="C10" t="inlineStr"/>
+      <c r="C10" t="n">
+        <v>45</v>
+      </c>
       <c r="D10" t="inlineStr">
         <is>
           <t>item B</t>
@@ -656,7 +674,9 @@
       <c r="B11" s="2" t="n">
         <v>44352</v>
       </c>
-      <c r="C11" t="inlineStr"/>
+      <c r="C11" t="n">
+        <v>50</v>
+      </c>
       <c r="D11" t="inlineStr">
         <is>
           <t>item A</t>
@@ -676,7 +696,9 @@
       <c r="B12" s="2" t="n">
         <v>44353</v>
       </c>
-      <c r="C12" t="inlineStr"/>
+      <c r="C12" t="n">
+        <v>60</v>
+      </c>
       <c r="D12" t="inlineStr">
         <is>
           <t>item B</t>
@@ -696,7 +718,9 @@
       <c r="B13" s="2" t="n">
         <v>44353</v>
       </c>
-      <c r="C13" t="inlineStr"/>
+      <c r="C13" t="n">
+        <v>80</v>
+      </c>
       <c r="D13" t="inlineStr">
         <is>
           <t>item C</t>
@@ -716,7 +740,9 @@
       <c r="B14" s="2" t="n">
         <v>44353</v>
       </c>
-      <c r="C14" t="inlineStr"/>
+      <c r="C14" t="n">
+        <v>60</v>
+      </c>
       <c r="D14" t="inlineStr">
         <is>
           <t>item B</t>
@@ -736,7 +762,9 @@
       <c r="B15" s="2" t="n">
         <v>44354</v>
       </c>
-      <c r="C15" t="inlineStr"/>
+      <c r="C15" t="n">
+        <v>15</v>
+      </c>
       <c r="D15" t="inlineStr">
         <is>
           <t>item B</t>
@@ -756,7 +784,9 @@
       <c r="B16" s="2" t="n">
         <v>44354</v>
       </c>
-      <c r="C16" t="inlineStr"/>
+      <c r="C16" t="n">
+        <v>20</v>
+      </c>
       <c r="D16" t="inlineStr">
         <is>
           <t>item A</t>
@@ -776,7 +806,9 @@
       <c r="B17" s="2" t="n">
         <v>44356</v>
       </c>
-      <c r="C17" t="inlineStr"/>
+      <c r="C17" t="n">
+        <v>10</v>
+      </c>
       <c r="D17" t="inlineStr">
         <is>
           <t>item A</t>
@@ -796,7 +828,9 @@
       <c r="B18" s="2" t="n">
         <v>44356</v>
       </c>
-      <c r="C18" t="inlineStr"/>
+      <c r="C18" t="n">
+        <v>20</v>
+      </c>
       <c r="D18" t="inlineStr">
         <is>
           <t>item C</t>
@@ -816,7 +850,9 @@
       <c r="B19" s="2" t="n">
         <v>44356</v>
       </c>
-      <c r="C19" t="inlineStr"/>
+      <c r="C19" t="n">
+        <v>75</v>
+      </c>
       <c r="D19" t="inlineStr">
         <is>
           <t>item B</t>
@@ -836,7 +872,9 @@
       <c r="B20" s="2" t="n">
         <v>44357</v>
       </c>
-      <c r="C20" t="inlineStr"/>
+      <c r="C20" t="n">
+        <v>80</v>
+      </c>
       <c r="D20" t="inlineStr">
         <is>
           <t>item C</t>
@@ -856,7 +894,9 @@
       <c r="B21" s="2" t="n">
         <v>44357</v>
       </c>
-      <c r="C21" t="inlineStr"/>
+      <c r="C21" t="n">
+        <v>100</v>
+      </c>
       <c r="D21" t="inlineStr">
         <is>
           <t>item D</t>
@@ -876,7 +916,9 @@
       <c r="B22" s="2" t="n">
         <v>44358</v>
       </c>
-      <c r="C22" t="inlineStr"/>
+      <c r="C22" t="n">
+        <v>125</v>
+      </c>
       <c r="D22" t="inlineStr">
         <is>
           <t>item D</t>
@@ -896,7 +938,9 @@
       <c r="B23" s="2" t="n">
         <v>44358</v>
       </c>
-      <c r="C23" t="inlineStr"/>
+      <c r="C23" t="n">
+        <v>30</v>
+      </c>
       <c r="D23" t="inlineStr">
         <is>
           <t>item B</t>
@@ -916,7 +960,9 @@
       <c r="B24" s="2" t="n">
         <v>44358</v>
       </c>
-      <c r="C24" t="inlineStr"/>
+      <c r="C24" t="n">
+        <v>125</v>
+      </c>
       <c r="D24" t="inlineStr">
         <is>
           <t>item D</t>
@@ -936,7 +982,9 @@
       <c r="B25" s="2" t="n">
         <v>44359</v>
       </c>
-      <c r="C25" t="inlineStr"/>
+      <c r="C25" t="n">
+        <v>45</v>
+      </c>
       <c r="D25" t="inlineStr">
         <is>
           <t>item B</t>
@@ -956,7 +1004,9 @@
       <c r="B26" s="2" t="n">
         <v>44359</v>
       </c>
-      <c r="C26" t="inlineStr"/>
+      <c r="C26" t="n">
+        <v>50</v>
+      </c>
       <c r="D26" t="inlineStr">
         <is>
           <t>item D</t>
@@ -976,7 +1026,9 @@
       <c r="B27" s="2" t="n">
         <v>44359</v>
       </c>
-      <c r="C27" t="inlineStr"/>
+      <c r="C27" t="n">
+        <v>10</v>
+      </c>
       <c r="D27" t="inlineStr">
         <is>
           <t>item A</t>
@@ -996,7 +1048,9 @@
       <c r="B28" s="2" t="n">
         <v>44360</v>
       </c>
-      <c r="C28" t="inlineStr"/>
+      <c r="C28" t="n">
+        <v>40</v>
+      </c>
       <c r="D28" t="inlineStr">
         <is>
           <t>item A</t>
@@ -1016,7 +1070,9 @@
       <c r="B29" s="2" t="n">
         <v>44360</v>
       </c>
-      <c r="C29" t="inlineStr"/>
+      <c r="C29" t="n">
+        <v>75</v>
+      </c>
       <c r="D29" t="inlineStr">
         <is>
           <t>item D</t>
@@ -1036,7 +1092,9 @@
       <c r="B30" s="2" t="n">
         <v>44360</v>
       </c>
-      <c r="C30" t="inlineStr"/>
+      <c r="C30" t="n">
+        <v>80</v>
+      </c>
       <c r="D30" t="inlineStr">
         <is>
           <t>item C</t>
@@ -1056,7 +1114,9 @@
       <c r="B31" s="2" t="n">
         <v>44360</v>
       </c>
-      <c r="C31" t="inlineStr"/>
+      <c r="C31" t="n">
+        <v>50</v>
+      </c>
       <c r="D31" t="inlineStr">
         <is>
           <t>item D</t>
@@ -1076,7 +1136,9 @@
       <c r="B32" s="2" t="n">
         <v>44360</v>
       </c>
-      <c r="C32" t="inlineStr"/>
+      <c r="C32" t="n">
+        <v>45</v>
+      </c>
       <c r="D32" t="inlineStr">
         <is>
           <t>item B</t>
@@ -1096,7 +1158,9 @@
       <c r="B33" s="2" t="n">
         <v>44360</v>
       </c>
-      <c r="C33" t="inlineStr"/>
+      <c r="C33" t="n">
+        <v>50</v>
+      </c>
       <c r="D33" t="inlineStr">
         <is>
           <t>item D</t>
@@ -1116,7 +1180,9 @@
       <c r="B34" s="2" t="n">
         <v>44361</v>
       </c>
-      <c r="C34" t="inlineStr"/>
+      <c r="C34" t="n">
+        <v>30</v>
+      </c>
       <c r="D34" t="inlineStr">
         <is>
           <t>item B</t>
@@ -1136,7 +1202,9 @@
       <c r="B35" s="2" t="n">
         <v>44361</v>
       </c>
-      <c r="C35" t="inlineStr"/>
+      <c r="C35" t="n">
+        <v>50</v>
+      </c>
       <c r="D35" t="inlineStr">
         <is>
           <t>item D</t>
@@ -1156,7 +1224,9 @@
       <c r="B36" s="2" t="n">
         <v>44362</v>
       </c>
-      <c r="C36" t="inlineStr"/>
+      <c r="C36" t="n">
+        <v>25</v>
+      </c>
       <c r="D36" t="inlineStr">
         <is>
           <t>item D</t>
@@ -1176,7 +1246,9 @@
       <c r="B37" s="2" t="n">
         <v>44362</v>
       </c>
-      <c r="C37" t="inlineStr"/>
+      <c r="C37" t="n">
+        <v>60</v>
+      </c>
       <c r="D37" t="inlineStr">
         <is>
           <t>item B</t>
@@ -1196,7 +1268,9 @@
       <c r="B38" s="2" t="n">
         <v>44362</v>
       </c>
-      <c r="C38" t="inlineStr"/>
+      <c r="C38" t="n">
+        <v>25</v>
+      </c>
       <c r="D38" t="inlineStr">
         <is>
           <t>item D</t>
@@ -1216,7 +1290,9 @@
       <c r="B39" s="2" t="n">
         <v>44365</v>
       </c>
-      <c r="C39" t="inlineStr"/>
+      <c r="C39" t="n">
+        <v>60</v>
+      </c>
       <c r="D39" t="inlineStr">
         <is>
           <t>item C</t>
@@ -1236,7 +1312,9 @@
       <c r="B40" s="2" t="n">
         <v>44365</v>
       </c>
-      <c r="C40" t="inlineStr"/>
+      <c r="C40" t="n">
+        <v>15</v>
+      </c>
       <c r="D40" t="inlineStr">
         <is>
           <t>item B</t>
@@ -1256,7 +1334,9 @@
       <c r="B41" s="2" t="n">
         <v>44365</v>
       </c>
-      <c r="C41" t="inlineStr"/>
+      <c r="C41" t="n">
+        <v>75</v>
+      </c>
       <c r="D41" t="inlineStr">
         <is>
           <t>item D</t>
@@ -1276,7 +1356,9 @@
       <c r="B42" s="2" t="n">
         <v>44365</v>
       </c>
-      <c r="C42" t="inlineStr"/>
+      <c r="C42" t="n">
+        <v>30</v>
+      </c>
       <c r="D42" t="inlineStr">
         <is>
           <t>item B</t>
@@ -1296,7 +1378,9 @@
       <c r="B43" s="2" t="n">
         <v>44365</v>
       </c>
-      <c r="C43" t="inlineStr"/>
+      <c r="C43" t="n">
+        <v>30</v>
+      </c>
       <c r="D43" t="inlineStr">
         <is>
           <t>item A</t>
@@ -1316,7 +1400,9 @@
       <c r="B44" s="2" t="n">
         <v>44366</v>
       </c>
-      <c r="C44" t="inlineStr"/>
+      <c r="C44" t="n">
+        <v>75</v>
+      </c>
       <c r="D44" t="inlineStr">
         <is>
           <t>item B</t>
@@ -1336,7 +1422,9 @@
       <c r="B45" s="2" t="n">
         <v>44366</v>
       </c>
-      <c r="C45" t="inlineStr"/>
+      <c r="C45" t="n">
+        <v>20</v>
+      </c>
       <c r="D45" t="inlineStr">
         <is>
           <t>item C</t>
@@ -1356,7 +1444,9 @@
       <c r="B46" s="2" t="n">
         <v>44366</v>
       </c>
-      <c r="C46" t="inlineStr"/>
+      <c r="C46" t="n">
+        <v>60</v>
+      </c>
       <c r="D46" t="inlineStr">
         <is>
           <t>item B</t>
@@ -1376,7 +1466,9 @@
       <c r="B47" s="2" t="n">
         <v>44367</v>
       </c>
-      <c r="C47" t="inlineStr"/>
+      <c r="C47" t="n">
+        <v>45</v>
+      </c>
       <c r="D47" t="inlineStr">
         <is>
           <t>item B</t>
@@ -1396,7 +1488,9 @@
       <c r="B48" s="2" t="n">
         <v>44367</v>
       </c>
-      <c r="C48" t="inlineStr"/>
+      <c r="C48" t="n">
+        <v>100</v>
+      </c>
       <c r="D48" t="inlineStr">
         <is>
           <t>item D</t>
@@ -1416,7 +1510,9 @@
       <c r="B49" s="2" t="n">
         <v>44367</v>
       </c>
-      <c r="C49" t="inlineStr"/>
+      <c r="C49" t="n">
+        <v>40</v>
+      </c>
       <c r="D49" t="inlineStr">
         <is>
           <t>item A</t>
@@ -1436,7 +1532,9 @@
       <c r="B50" s="2" t="n">
         <v>44367</v>
       </c>
-      <c r="C50" t="inlineStr"/>
+      <c r="C50" t="n">
+        <v>50</v>
+      </c>
       <c r="D50" t="inlineStr">
         <is>
           <t>item D</t>
@@ -1456,7 +1554,9 @@
       <c r="B51" s="2" t="n">
         <v>44367</v>
       </c>
-      <c r="C51" t="inlineStr"/>
+      <c r="C51" t="n">
+        <v>10</v>
+      </c>
       <c r="D51" t="inlineStr">
         <is>
           <t>item A</t>
@@ -1476,7 +1576,9 @@
       <c r="B52" s="2" t="n">
         <v>44367</v>
       </c>
-      <c r="C52" t="inlineStr"/>
+      <c r="C52" t="n">
+        <v>75</v>
+      </c>
       <c r="D52" t="inlineStr">
         <is>
           <t>item B</t>
@@ -1496,7 +1598,9 @@
       <c r="B53" s="2" t="n">
         <v>44369</v>
       </c>
-      <c r="C53" t="inlineStr"/>
+      <c r="C53" t="n">
+        <v>40</v>
+      </c>
       <c r="D53" t="inlineStr">
         <is>
           <t>item A</t>
@@ -1516,7 +1620,9 @@
       <c r="B54" s="2" t="n">
         <v>44369</v>
       </c>
-      <c r="C54" t="inlineStr"/>
+      <c r="C54" t="n">
+        <v>40</v>
+      </c>
       <c r="D54" t="inlineStr">
         <is>
           <t>item C</t>
@@ -1536,7 +1642,9 @@
       <c r="B55" s="2" t="n">
         <v>44369</v>
       </c>
-      <c r="C55" t="inlineStr"/>
+      <c r="C55" t="n">
+        <v>40</v>
+      </c>
       <c r="D55" t="inlineStr">
         <is>
           <t>item A</t>
@@ -1556,7 +1664,9 @@
       <c r="B56" s="2" t="n">
         <v>44370</v>
       </c>
-      <c r="C56" t="inlineStr"/>
+      <c r="C56" t="n">
+        <v>20</v>
+      </c>
       <c r="D56" t="inlineStr">
         <is>
           <t>item C</t>
@@ -1576,7 +1686,9 @@
       <c r="B57" s="2" t="n">
         <v>44370</v>
       </c>
-      <c r="C57" t="inlineStr"/>
+      <c r="C57" t="n">
+        <v>50</v>
+      </c>
       <c r="D57" t="inlineStr">
         <is>
           <t>item A</t>
@@ -1596,7 +1708,9 @@
       <c r="B58" s="2" t="n">
         <v>44370</v>
       </c>
-      <c r="C58" t="inlineStr"/>
+      <c r="C58" t="n">
+        <v>100</v>
+      </c>
       <c r="D58" t="inlineStr">
         <is>
           <t>item D</t>
@@ -1616,7 +1730,9 @@
       <c r="B59" s="2" t="n">
         <v>44372</v>
       </c>
-      <c r="C59" t="inlineStr"/>
+      <c r="C59" t="n">
+        <v>20</v>
+      </c>
       <c r="D59" t="inlineStr">
         <is>
           <t>item A</t>
@@ -1636,7 +1752,9 @@
       <c r="B60" s="2" t="n">
         <v>44372</v>
       </c>
-      <c r="C60" t="inlineStr"/>
+      <c r="C60" t="n">
+        <v>45</v>
+      </c>
       <c r="D60" t="inlineStr">
         <is>
           <t>item B</t>
@@ -1656,7 +1774,9 @@
       <c r="B61" s="2" t="n">
         <v>44372</v>
       </c>
-      <c r="C61" t="inlineStr"/>
+      <c r="C61" t="n">
+        <v>20</v>
+      </c>
       <c r="D61" t="inlineStr">
         <is>
           <t>item C</t>
@@ -1676,7 +1796,9 @@
       <c r="B62" s="2" t="n">
         <v>44372</v>
       </c>
-      <c r="C62" t="inlineStr"/>
+      <c r="C62" t="n">
+        <v>75</v>
+      </c>
       <c r="D62" t="inlineStr">
         <is>
           <t>item B</t>
@@ -1696,7 +1818,9 @@
       <c r="B63" s="2" t="n">
         <v>44372</v>
       </c>
-      <c r="C63" t="inlineStr"/>
+      <c r="C63" t="n">
+        <v>100</v>
+      </c>
       <c r="D63" t="inlineStr">
         <is>
           <t>item D</t>
@@ -1716,7 +1840,9 @@
       <c r="B64" s="2" t="n">
         <v>44373</v>
       </c>
-      <c r="C64" t="inlineStr"/>
+      <c r="C64" t="n">
+        <v>20</v>
+      </c>
       <c r="D64" t="inlineStr">
         <is>
           <t>item A</t>
@@ -1736,7 +1862,9 @@
       <c r="B65" s="2" t="n">
         <v>44373</v>
       </c>
-      <c r="C65" t="inlineStr"/>
+      <c r="C65" t="n">
+        <v>15</v>
+      </c>
       <c r="D65" t="inlineStr">
         <is>
           <t>item B</t>
@@ -1756,7 +1884,9 @@
       <c r="B66" s="2" t="n">
         <v>44373</v>
       </c>
-      <c r="C66" t="inlineStr"/>
+      <c r="C66" t="n">
+        <v>80</v>
+      </c>
       <c r="D66" t="inlineStr">
         <is>
           <t>item C</t>
@@ -1776,7 +1906,9 @@
       <c r="B67" s="2" t="n">
         <v>44373</v>
       </c>
-      <c r="C67" t="inlineStr"/>
+      <c r="C67" t="n">
+        <v>100</v>
+      </c>
       <c r="D67" t="inlineStr">
         <is>
           <t>item D</t>
@@ -1796,7 +1928,9 @@
       <c r="B68" s="2" t="n">
         <v>44373</v>
       </c>
-      <c r="C68" t="inlineStr"/>
+      <c r="C68" t="n">
+        <v>50</v>
+      </c>
       <c r="D68" t="inlineStr">
         <is>
           <t>item A</t>
@@ -1816,7 +1950,9 @@
       <c r="B69" s="2" t="n">
         <v>44373</v>
       </c>
-      <c r="C69" t="inlineStr"/>
+      <c r="C69" t="n">
+        <v>100</v>
+      </c>
       <c r="D69" t="inlineStr">
         <is>
           <t>item C</t>
@@ -1836,7 +1972,9 @@
       <c r="B70" s="2" t="n">
         <v>44374</v>
       </c>
-      <c r="C70" t="inlineStr"/>
+      <c r="C70" t="n">
+        <v>15</v>
+      </c>
       <c r="D70" t="inlineStr">
         <is>
           <t>item B</t>
@@ -1856,7 +1994,9 @@
       <c r="B71" s="2" t="n">
         <v>44374</v>
       </c>
-      <c r="C71" t="inlineStr"/>
+      <c r="C71" t="n">
+        <v>75</v>
+      </c>
       <c r="D71" t="inlineStr">
         <is>
           <t>item D</t>
@@ -1876,7 +2016,9 @@
       <c r="B72" s="2" t="n">
         <v>44374</v>
       </c>
-      <c r="C72" t="inlineStr"/>
+      <c r="C72" t="n">
+        <v>20</v>
+      </c>
       <c r="D72" t="inlineStr">
         <is>
           <t>item A</t>
@@ -1896,7 +2038,9 @@
       <c r="B73" s="2" t="n">
         <v>44374</v>
       </c>
-      <c r="C73" t="inlineStr"/>
+      <c r="C73" t="n">
+        <v>20</v>
+      </c>
       <c r="D73" t="inlineStr">
         <is>
           <t>item C</t>
@@ -1916,7 +2060,9 @@
       <c r="B74" s="2" t="n">
         <v>44374</v>
       </c>
-      <c r="C74" t="inlineStr"/>
+      <c r="C74" t="n">
+        <v>10</v>
+      </c>
       <c r="D74" t="inlineStr">
         <is>
           <t>item A</t>
@@ -1936,7 +2082,9 @@
       <c r="B75" s="2" t="n">
         <v>44374</v>
       </c>
-      <c r="C75" t="inlineStr"/>
+      <c r="C75" t="n">
+        <v>40</v>
+      </c>
       <c r="D75" t="inlineStr">
         <is>
           <t>item C</t>
@@ -1956,7 +2104,9 @@
       <c r="B76" s="2" t="n">
         <v>44375</v>
       </c>
-      <c r="C76" t="inlineStr"/>
+      <c r="C76" t="n">
+        <v>15</v>
+      </c>
       <c r="D76" t="inlineStr">
         <is>
           <t>item B</t>
@@ -1976,7 +2126,9 @@
       <c r="B77" s="2" t="n">
         <v>44375</v>
       </c>
-      <c r="C77" t="inlineStr"/>
+      <c r="C77" t="n">
+        <v>50</v>
+      </c>
       <c r="D77" t="inlineStr">
         <is>
           <t>item A</t>
@@ -1996,7 +2148,9 @@
       <c r="B78" s="2" t="n">
         <v>44376</v>
       </c>
-      <c r="C78" t="inlineStr"/>
+      <c r="C78" t="n">
+        <v>75</v>
+      </c>
       <c r="D78" t="inlineStr">
         <is>
           <t>item D</t>
@@ -2016,7 +2170,9 @@
       <c r="B79" s="2" t="n">
         <v>44376</v>
       </c>
-      <c r="C79" t="inlineStr"/>
+      <c r="C79" t="n">
+        <v>100</v>
+      </c>
       <c r="D79" t="inlineStr">
         <is>
           <t>item C</t>
@@ -2036,7 +2192,9 @@
       <c r="B80" s="2" t="n">
         <v>44376</v>
       </c>
-      <c r="C80" t="inlineStr"/>
+      <c r="C80" t="n">
+        <v>100</v>
+      </c>
       <c r="D80" t="inlineStr">
         <is>
           <t>item D</t>
@@ -2056,7 +2214,9 @@
       <c r="B81" s="2" t="n">
         <v>44377</v>
       </c>
-      <c r="C81" t="inlineStr"/>
+      <c r="C81" t="n">
+        <v>30</v>
+      </c>
       <c r="D81" t="inlineStr">
         <is>
           <t>item B</t>
@@ -2076,7 +2236,9 @@
       <c r="B82" s="2" t="n">
         <v>44377</v>
       </c>
-      <c r="C82" t="inlineStr"/>
+      <c r="C82" t="n">
+        <v>100</v>
+      </c>
       <c r="D82" t="inlineStr">
         <is>
           <t>item D</t>
@@ -2096,7 +2258,9 @@
       <c r="B83" s="2" t="n">
         <v>44377</v>
       </c>
-      <c r="C83" t="inlineStr"/>
+      <c r="C83" t="n">
+        <v>75</v>
+      </c>
       <c r="D83" t="inlineStr">
         <is>
           <t>item B</t>
@@ -2116,7 +2280,9 @@
       <c r="B84" s="2" t="n">
         <v>44378</v>
       </c>
-      <c r="C84" t="inlineStr"/>
+      <c r="C84" t="n">
+        <v>60</v>
+      </c>
       <c r="D84" t="inlineStr">
         <is>
           <t>item C</t>
@@ -2136,7 +2302,9 @@
       <c r="B85" s="2" t="n">
         <v>44378</v>
       </c>
-      <c r="C85" t="inlineStr"/>
+      <c r="C85" t="n">
+        <v>50</v>
+      </c>
       <c r="D85" t="inlineStr">
         <is>
           <t>item A</t>
@@ -2156,7 +2324,9 @@
       <c r="B86" s="2" t="n">
         <v>44379</v>
       </c>
-      <c r="C86" t="inlineStr"/>
+      <c r="C86" t="n">
+        <v>60</v>
+      </c>
       <c r="D86" t="inlineStr">
         <is>
           <t>item B</t>
@@ -2176,7 +2346,9 @@
       <c r="B87" s="2" t="n">
         <v>44379</v>
       </c>
-      <c r="C87" t="inlineStr"/>
+      <c r="C87" t="n">
+        <v>20</v>
+      </c>
       <c r="D87" t="inlineStr">
         <is>
           <t>item A</t>
@@ -2196,7 +2368,9 @@
       <c r="B88" s="2" t="n">
         <v>44379</v>
       </c>
-      <c r="C88" t="inlineStr"/>
+      <c r="C88" t="n">
+        <v>20</v>
+      </c>
       <c r="D88" t="inlineStr">
         <is>
           <t>item C</t>
@@ -2216,7 +2390,9 @@
       <c r="B89" s="2" t="n">
         <v>44379</v>
       </c>
-      <c r="C89" t="inlineStr"/>
+      <c r="C89" t="n">
+        <v>75</v>
+      </c>
       <c r="D89" t="inlineStr">
         <is>
           <t>item D</t>
@@ -2236,7 +2412,9 @@
       <c r="B90" s="2" t="n">
         <v>44380</v>
       </c>
-      <c r="C90" t="inlineStr"/>
+      <c r="C90" t="n">
+        <v>40</v>
+      </c>
       <c r="D90" t="inlineStr">
         <is>
           <t>item C</t>
@@ -2256,7 +2434,9 @@
       <c r="B91" s="2" t="n">
         <v>44380</v>
       </c>
-      <c r="C91" t="inlineStr"/>
+      <c r="C91" t="n">
+        <v>50</v>
+      </c>
       <c r="D91" t="inlineStr">
         <is>
           <t>item D</t>
@@ -2276,7 +2456,9 @@
       <c r="B92" s="2" t="n">
         <v>44380</v>
       </c>
-      <c r="C92" t="inlineStr"/>
+      <c r="C92" t="n">
+        <v>60</v>
+      </c>
       <c r="D92" t="inlineStr">
         <is>
           <t>item B</t>
@@ -2296,7 +2478,9 @@
       <c r="B93" s="2" t="n">
         <v>44380</v>
       </c>
-      <c r="C93" t="inlineStr"/>
+      <c r="C93" t="n">
+        <v>125</v>
+      </c>
       <c r="D93" t="inlineStr">
         <is>
           <t>item D</t>
@@ -2316,7 +2500,9 @@
       <c r="B94" s="2" t="n">
         <v>44380</v>
       </c>
-      <c r="C94" t="inlineStr"/>
+      <c r="C94" t="n">
+        <v>100</v>
+      </c>
       <c r="D94" t="inlineStr">
         <is>
           <t>item C</t>
@@ -2336,7 +2522,9 @@
       <c r="B95" s="2" t="n">
         <v>44380</v>
       </c>
-      <c r="C95" t="inlineStr"/>
+      <c r="C95" t="n">
+        <v>75</v>
+      </c>
       <c r="D95" t="inlineStr">
         <is>
           <t>item B</t>
@@ -2356,7 +2544,9 @@
       <c r="B96" s="2" t="n">
         <v>44381</v>
       </c>
-      <c r="C96" t="inlineStr"/>
+      <c r="C96" t="n">
+        <v>30</v>
+      </c>
       <c r="D96" t="inlineStr">
         <is>
           <t>item A</t>
@@ -2376,7 +2566,9 @@
       <c r="B97" s="2" t="n">
         <v>44381</v>
       </c>
-      <c r="C97" t="inlineStr"/>
+      <c r="C97" t="n">
+        <v>50</v>
+      </c>
       <c r="D97" t="inlineStr">
         <is>
           <t>item D</t>
@@ -2396,7 +2588,9 @@
       <c r="B98" s="2" t="n">
         <v>44381</v>
       </c>
-      <c r="C98" t="inlineStr"/>
+      <c r="C98" t="n">
+        <v>45</v>
+      </c>
       <c r="D98" t="inlineStr">
         <is>
           <t>item B</t>
@@ -2416,7 +2610,9 @@
       <c r="B99" s="2" t="n">
         <v>44382</v>
       </c>
-      <c r="C99" t="inlineStr"/>
+      <c r="C99" t="n">
+        <v>15</v>
+      </c>
       <c r="D99" t="inlineStr">
         <is>
           <t>item B</t>
@@ -2436,7 +2632,9 @@
       <c r="B100" s="2" t="n">
         <v>44382</v>
       </c>
-      <c r="C100" t="inlineStr"/>
+      <c r="C100" t="n">
+        <v>40</v>
+      </c>
       <c r="D100" t="inlineStr">
         <is>
           <t>item A</t>
@@ -2456,7 +2654,9 @@
       <c r="B101" s="2" t="n">
         <v>44382</v>
       </c>
-      <c r="C101" t="inlineStr"/>
+      <c r="C101" t="n">
+        <v>50</v>
+      </c>
       <c r="D101" t="inlineStr">
         <is>
           <t>item D</t>
@@ -2476,7 +2676,9 @@
       <c r="B102" s="2" t="n">
         <v>44383</v>
       </c>
-      <c r="C102" t="inlineStr"/>
+      <c r="C102" t="n">
+        <v>45</v>
+      </c>
       <c r="D102" t="inlineStr">
         <is>
           <t>item B</t>
@@ -2496,7 +2698,9 @@
       <c r="B103" s="2" t="n">
         <v>44383</v>
       </c>
-      <c r="C103" t="inlineStr"/>
+      <c r="C103" t="n">
+        <v>100</v>
+      </c>
       <c r="D103" t="inlineStr">
         <is>
           <t>item C</t>
@@ -2516,7 +2720,9 @@
       <c r="B104" s="2" t="n">
         <v>44383</v>
       </c>
-      <c r="C104" t="inlineStr"/>
+      <c r="C104" t="n">
+        <v>25</v>
+      </c>
       <c r="D104" t="inlineStr">
         <is>
           <t>item D</t>
@@ -2536,7 +2742,9 @@
       <c r="B105" s="2" t="n">
         <v>44383</v>
       </c>
-      <c r="C105" t="inlineStr"/>
+      <c r="C105" t="n">
+        <v>20</v>
+      </c>
       <c r="D105" t="inlineStr">
         <is>
           <t>item C</t>
@@ -2556,7 +2764,9 @@
       <c r="B106" s="2" t="n">
         <v>44384</v>
       </c>
-      <c r="C106" t="inlineStr"/>
+      <c r="C106" t="n">
+        <v>50</v>
+      </c>
       <c r="D106" t="inlineStr">
         <is>
           <t>item A</t>
@@ -2576,7 +2786,9 @@
       <c r="B107" s="2" t="n">
         <v>44384</v>
       </c>
-      <c r="C107" t="inlineStr"/>
+      <c r="C107" t="n">
+        <v>60</v>
+      </c>
       <c r="D107" t="inlineStr">
         <is>
           <t>item B</t>
@@ -2596,7 +2808,9 @@
       <c r="B108" s="2" t="n">
         <v>44384</v>
       </c>
-      <c r="C108" t="inlineStr"/>
+      <c r="C108" t="n">
+        <v>80</v>
+      </c>
       <c r="D108" t="inlineStr">
         <is>
           <t>item C</t>
@@ -2616,7 +2830,9 @@
       <c r="B109" s="2" t="n">
         <v>44385</v>
       </c>
-      <c r="C109" t="inlineStr"/>
+      <c r="C109" t="n">
+        <v>40</v>
+      </c>
       <c r="D109" t="inlineStr">
         <is>
           <t>item A</t>
@@ -2636,7 +2852,9 @@
       <c r="B110" s="2" t="n">
         <v>44385</v>
       </c>
-      <c r="C110" t="inlineStr"/>
+      <c r="C110" t="n">
+        <v>75</v>
+      </c>
       <c r="D110" t="inlineStr">
         <is>
           <t>item D</t>
@@ -2656,7 +2874,9 @@
       <c r="B111" s="2" t="n">
         <v>44385</v>
       </c>
-      <c r="C111" t="inlineStr"/>
+      <c r="C111" t="n">
+        <v>30</v>
+      </c>
       <c r="D111" t="inlineStr">
         <is>
           <t>item B</t>
@@ -2676,7 +2896,9 @@
       <c r="B112" s="2" t="n">
         <v>44386</v>
       </c>
-      <c r="C112" t="inlineStr"/>
+      <c r="C112" t="n">
+        <v>15</v>
+      </c>
       <c r="D112" t="inlineStr">
         <is>
           <t>item B</t>
@@ -2696,7 +2918,9 @@
       <c r="B113" s="2" t="n">
         <v>44386</v>
       </c>
-      <c r="C113" t="inlineStr"/>
+      <c r="C113" t="n">
+        <v>125</v>
+      </c>
       <c r="D113" t="inlineStr">
         <is>
           <t>item D</t>
@@ -2716,7 +2940,9 @@
       <c r="B114" s="2" t="n">
         <v>44386</v>
       </c>
-      <c r="C114" t="inlineStr"/>
+      <c r="C114" t="n">
+        <v>30</v>
+      </c>
       <c r="D114" t="inlineStr">
         <is>
           <t>item B</t>
@@ -2736,7 +2962,9 @@
       <c r="B115" s="2" t="n">
         <v>44386</v>
       </c>
-      <c r="C115" t="inlineStr"/>
+      <c r="C115" t="n">
+        <v>100</v>
+      </c>
       <c r="D115" t="inlineStr">
         <is>
           <t>item D</t>
@@ -2756,7 +2984,9 @@
       <c r="B116" s="2" t="n">
         <v>44386</v>
       </c>
-      <c r="C116" t="inlineStr"/>
+      <c r="C116" t="n">
+        <v>60</v>
+      </c>
       <c r="D116" t="inlineStr">
         <is>
           <t>item C</t>
@@ -2776,7 +3006,9 @@
       <c r="B117" s="2" t="n">
         <v>44387</v>
       </c>
-      <c r="C117" t="inlineStr"/>
+      <c r="C117" t="n">
+        <v>60</v>
+      </c>
       <c r="D117" t="inlineStr">
         <is>
           <t>item C</t>
@@ -2796,7 +3028,9 @@
       <c r="B118" s="2" t="n">
         <v>44387</v>
       </c>
-      <c r="C118" t="inlineStr"/>
+      <c r="C118" t="n">
+        <v>45</v>
+      </c>
       <c r="D118" t="inlineStr">
         <is>
           <t>item B</t>
@@ -2816,7 +3050,9 @@
       <c r="B119" s="2" t="n">
         <v>44387</v>
       </c>
-      <c r="C119" t="inlineStr"/>
+      <c r="C119" t="n">
+        <v>50</v>
+      </c>
       <c r="D119" t="inlineStr">
         <is>
           <t>item D</t>
@@ -2836,7 +3072,9 @@
       <c r="B120" s="2" t="n">
         <v>44387</v>
       </c>
-      <c r="C120" t="inlineStr"/>
+      <c r="C120" t="n">
+        <v>75</v>
+      </c>
       <c r="D120" t="inlineStr">
         <is>
           <t>item B</t>
@@ -2856,7 +3094,9 @@
       <c r="B121" s="2" t="n">
         <v>44387</v>
       </c>
-      <c r="C121" t="inlineStr"/>
+      <c r="C121" t="n">
+        <v>40</v>
+      </c>
       <c r="D121" t="inlineStr">
         <is>
           <t>item A</t>
@@ -2876,7 +3116,9 @@
       <c r="B122" s="2" t="n">
         <v>44387</v>
       </c>
-      <c r="C122" t="inlineStr"/>
+      <c r="C122" t="n">
+        <v>60</v>
+      </c>
       <c r="D122" t="inlineStr">
         <is>
           <t>item C</t>
@@ -2896,7 +3138,9 @@
       <c r="B123" s="2" t="n">
         <v>44388</v>
       </c>
-      <c r="C123" t="inlineStr"/>
+      <c r="C123" t="n">
+        <v>100</v>
+      </c>
       <c r="D123" t="inlineStr">
         <is>
           <t>item D</t>
@@ -2916,7 +3160,9 @@
       <c r="B124" s="2" t="n">
         <v>44388</v>
       </c>
-      <c r="C124" t="inlineStr"/>
+      <c r="C124" t="n">
+        <v>60</v>
+      </c>
       <c r="D124" t="inlineStr">
         <is>
           <t>item B</t>
@@ -2936,7 +3182,9 @@
       <c r="B125" s="2" t="n">
         <v>44388</v>
       </c>
-      <c r="C125" t="inlineStr"/>
+      <c r="C125" t="n">
+        <v>50</v>
+      </c>
       <c r="D125" t="inlineStr">
         <is>
           <t>item D</t>
@@ -2956,7 +3204,9 @@
       <c r="B126" s="2" t="n">
         <v>44388</v>
       </c>
-      <c r="C126" t="inlineStr"/>
+      <c r="C126" t="n">
+        <v>60</v>
+      </c>
       <c r="D126" t="inlineStr">
         <is>
           <t>item B</t>
@@ -2976,7 +3226,9 @@
       <c r="B127" s="2" t="n">
         <v>44388</v>
       </c>
-      <c r="C127" t="inlineStr"/>
+      <c r="C127" t="n">
+        <v>40</v>
+      </c>
       <c r="D127" t="inlineStr">
         <is>
           <t>item A</t>
@@ -2996,7 +3248,9 @@
       <c r="B128" s="2" t="n">
         <v>44389</v>
       </c>
-      <c r="C128" t="inlineStr"/>
+      <c r="C128" t="n">
+        <v>125</v>
+      </c>
       <c r="D128" t="inlineStr">
         <is>
           <t>item D</t>
@@ -3016,7 +3270,9 @@
       <c r="B129" s="2" t="n">
         <v>44389</v>
       </c>
-      <c r="C129" t="inlineStr"/>
+      <c r="C129" t="n">
+        <v>75</v>
+      </c>
       <c r="D129" t="inlineStr">
         <is>
           <t>item B</t>
@@ -3036,7 +3292,9 @@
       <c r="B130" s="2" t="n">
         <v>44389</v>
       </c>
-      <c r="C130" t="inlineStr"/>
+      <c r="C130" t="n">
+        <v>10</v>
+      </c>
       <c r="D130" t="inlineStr">
         <is>
           <t>item A</t>
@@ -3056,7 +3314,9 @@
       <c r="B131" s="2" t="n">
         <v>44390</v>
       </c>
-      <c r="C131" t="inlineStr"/>
+      <c r="C131" t="n">
+        <v>45</v>
+      </c>
       <c r="D131" t="inlineStr">
         <is>
           <t>item B</t>
@@ -3076,7 +3336,9 @@
       <c r="B132" s="2" t="n">
         <v>44390</v>
       </c>
-      <c r="C132" t="inlineStr"/>
+      <c r="C132" t="n">
+        <v>80</v>
+      </c>
       <c r="D132" t="inlineStr">
         <is>
           <t>item C</t>
@@ -3096,7 +3358,9 @@
       <c r="B133" s="2" t="n">
         <v>44391</v>
       </c>
-      <c r="C133" t="inlineStr"/>
+      <c r="C133" t="n">
+        <v>50</v>
+      </c>
       <c r="D133" t="inlineStr">
         <is>
           <t>item D</t>
@@ -3116,7 +3380,9 @@
       <c r="B134" s="2" t="n">
         <v>44391</v>
       </c>
-      <c r="C134" t="inlineStr"/>
+      <c r="C134" t="n">
+        <v>40</v>
+      </c>
       <c r="D134" t="inlineStr">
         <is>
           <t>item A</t>
@@ -3136,7 +3402,9 @@
       <c r="B135" s="2" t="n">
         <v>44391</v>
       </c>
-      <c r="C135" t="inlineStr"/>
+      <c r="C135" t="n">
+        <v>100</v>
+      </c>
       <c r="D135" t="inlineStr">
         <is>
           <t>item D</t>
@@ -3156,7 +3424,9 @@
       <c r="B136" s="2" t="n">
         <v>44392</v>
       </c>
-      <c r="C136" t="inlineStr"/>
+      <c r="C136" t="n">
+        <v>25</v>
+      </c>
       <c r="D136" t="inlineStr">
         <is>
           <t>item D</t>
@@ -3176,7 +3446,9 @@
       <c r="B137" s="2" t="n">
         <v>44392</v>
       </c>
-      <c r="C137" t="inlineStr"/>
+      <c r="C137" t="n">
+        <v>10</v>
+      </c>
       <c r="D137" t="inlineStr">
         <is>
           <t>item A</t>
@@ -3196,7 +3468,9 @@
       <c r="B138" s="2" t="n">
         <v>44392</v>
       </c>
-      <c r="C138" t="inlineStr"/>
+      <c r="C138" t="n">
+        <v>100</v>
+      </c>
       <c r="D138" t="inlineStr">
         <is>
           <t>item D</t>
@@ -3216,7 +3490,9 @@
       <c r="B139" s="2" t="n">
         <v>44393</v>
       </c>
-      <c r="C139" t="inlineStr"/>
+      <c r="C139" t="n">
+        <v>40</v>
+      </c>
       <c r="D139" t="inlineStr">
         <is>
           <t>item C</t>
@@ -3236,7 +3512,9 @@
       <c r="B140" s="2" t="n">
         <v>44393</v>
       </c>
-      <c r="C140" t="inlineStr"/>
+      <c r="C140" t="n">
+        <v>50</v>
+      </c>
       <c r="D140" t="inlineStr">
         <is>
           <t>item A</t>
@@ -3256,7 +3534,9 @@
       <c r="B141" s="2" t="n">
         <v>44393</v>
       </c>
-      <c r="C141" t="inlineStr"/>
+      <c r="C141" t="n">
+        <v>60</v>
+      </c>
       <c r="D141" t="inlineStr">
         <is>
           <t>item C</t>
@@ -3276,7 +3556,9 @@
       <c r="B142" s="2" t="n">
         <v>44394</v>
       </c>
-      <c r="C142" t="inlineStr"/>
+      <c r="C142" t="n">
+        <v>60</v>
+      </c>
       <c r="D142" t="inlineStr">
         <is>
           <t>item B</t>
@@ -3296,7 +3578,9 @@
       <c r="B143" s="2" t="n">
         <v>44394</v>
       </c>
-      <c r="C143" t="inlineStr"/>
+      <c r="C143" t="n">
+        <v>40</v>
+      </c>
       <c r="D143" t="inlineStr">
         <is>
           <t>item C</t>
@@ -3316,7 +3600,9 @@
       <c r="B144" s="2" t="n">
         <v>44394</v>
       </c>
-      <c r="C144" t="inlineStr"/>
+      <c r="C144" t="n">
+        <v>100</v>
+      </c>
       <c r="D144" t="inlineStr">
         <is>
           <t>item D</t>
@@ -3336,7 +3622,9 @@
       <c r="B145" s="2" t="n">
         <v>44394</v>
       </c>
-      <c r="C145" t="inlineStr"/>
+      <c r="C145" t="n">
+        <v>50</v>
+      </c>
       <c r="D145" t="inlineStr">
         <is>
           <t>item A</t>
@@ -3356,7 +3644,9 @@
       <c r="B146" s="2" t="n">
         <v>44394</v>
       </c>
-      <c r="C146" t="inlineStr"/>
+      <c r="C146" t="n">
+        <v>20</v>
+      </c>
       <c r="D146" t="inlineStr">
         <is>
           <t>item C</t>
@@ -3376,7 +3666,9 @@
       <c r="B147" s="2" t="n">
         <v>44394</v>
       </c>
-      <c r="C147" t="inlineStr"/>
+      <c r="C147" t="n">
+        <v>15</v>
+      </c>
       <c r="D147" t="inlineStr">
         <is>
           <t>item B</t>
@@ -3396,7 +3688,9 @@
       <c r="B148" s="2" t="n">
         <v>44395</v>
       </c>
-      <c r="C148" t="inlineStr"/>
+      <c r="C148" t="n">
+        <v>20</v>
+      </c>
       <c r="D148" t="inlineStr">
         <is>
           <t>item A</t>
@@ -3416,7 +3710,9 @@
       <c r="B149" s="2" t="n">
         <v>44395</v>
       </c>
-      <c r="C149" t="inlineStr"/>
+      <c r="C149" t="n">
+        <v>25</v>
+      </c>
       <c r="D149" t="inlineStr">
         <is>
           <t>item D</t>
@@ -3436,7 +3732,9 @@
       <c r="B150" s="2" t="n">
         <v>44395</v>
       </c>
-      <c r="C150" t="inlineStr"/>
+      <c r="C150" t="n">
+        <v>30</v>
+      </c>
       <c r="D150" t="inlineStr">
         <is>
           <t>item B</t>
@@ -3456,7 +3754,9 @@
       <c r="B151" s="2" t="n">
         <v>44395</v>
       </c>
-      <c r="C151" t="inlineStr"/>
+      <c r="C151" t="n">
+        <v>100</v>
+      </c>
       <c r="D151" t="inlineStr">
         <is>
           <t>item C</t>
@@ -3476,7 +3776,9 @@
       <c r="B152" s="2" t="n">
         <v>44395</v>
       </c>
-      <c r="C152" t="inlineStr"/>
+      <c r="C152" t="n">
+        <v>20</v>
+      </c>
       <c r="D152" t="inlineStr">
         <is>
           <t>item A</t>
@@ -3496,7 +3798,9 @@
       <c r="B153" s="2" t="n">
         <v>44395</v>
       </c>
-      <c r="C153" t="inlineStr"/>
+      <c r="C153" t="n">
+        <v>20</v>
+      </c>
       <c r="D153" t="inlineStr">
         <is>
           <t>item C</t>
@@ -3516,7 +3820,9 @@
       <c r="B154" s="2" t="n">
         <v>44396</v>
       </c>
-      <c r="C154" t="inlineStr"/>
+      <c r="C154" t="n">
+        <v>100</v>
+      </c>
       <c r="D154" t="inlineStr">
         <is>
           <t>item C</t>
@@ -3536,7 +3842,9 @@
       <c r="B155" s="2" t="n">
         <v>44396</v>
       </c>
-      <c r="C155" t="inlineStr"/>
+      <c r="C155" t="n">
+        <v>75</v>
+      </c>
       <c r="D155" t="inlineStr">
         <is>
           <t>item D</t>
@@ -3556,7 +3864,9 @@
       <c r="B156" s="2" t="n">
         <v>44397</v>
       </c>
-      <c r="C156" t="inlineStr"/>
+      <c r="C156" t="n">
+        <v>100</v>
+      </c>
       <c r="D156" t="inlineStr">
         <is>
           <t>item C</t>
@@ -3576,7 +3886,9 @@
       <c r="B157" s="2" t="n">
         <v>44397</v>
       </c>
-      <c r="C157" t="inlineStr"/>
+      <c r="C157" t="n">
+        <v>100</v>
+      </c>
       <c r="D157" t="inlineStr">
         <is>
           <t>item D</t>
@@ -3596,7 +3908,9 @@
       <c r="B158" s="2" t="n">
         <v>44397</v>
       </c>
-      <c r="C158" t="inlineStr"/>
+      <c r="C158" t="n">
+        <v>60</v>
+      </c>
       <c r="D158" t="inlineStr">
         <is>
           <t>item C</t>
@@ -3616,7 +3930,9 @@
       <c r="B159" s="2" t="n">
         <v>44398</v>
       </c>
-      <c r="C159" t="inlineStr"/>
+      <c r="C159" t="n">
+        <v>50</v>
+      </c>
       <c r="D159" t="inlineStr">
         <is>
           <t>item D</t>
@@ -3636,7 +3952,9 @@
       <c r="B160" s="2" t="n">
         <v>44398</v>
       </c>
-      <c r="C160" t="inlineStr"/>
+      <c r="C160" t="n">
+        <v>100</v>
+      </c>
       <c r="D160" t="inlineStr">
         <is>
           <t>item C</t>
@@ -3656,7 +3974,9 @@
       <c r="B161" s="2" t="n">
         <v>44399</v>
       </c>
-      <c r="C161" t="inlineStr"/>
+      <c r="C161" t="n">
+        <v>75</v>
+      </c>
       <c r="D161" t="inlineStr">
         <is>
           <t>item D</t>
@@ -3676,7 +3996,9 @@
       <c r="B162" s="2" t="n">
         <v>44399</v>
       </c>
-      <c r="C162" t="inlineStr"/>
+      <c r="C162" t="n">
+        <v>30</v>
+      </c>
       <c r="D162" t="inlineStr">
         <is>
           <t>item A</t>
@@ -3696,7 +4018,9 @@
       <c r="B163" s="2" t="n">
         <v>44399</v>
       </c>
-      <c r="C163" t="inlineStr"/>
+      <c r="C163" t="n">
+        <v>60</v>
+      </c>
       <c r="D163" t="inlineStr">
         <is>
           <t>item C</t>
@@ -3716,7 +4040,9 @@
       <c r="B164" s="2" t="n">
         <v>44400</v>
       </c>
-      <c r="C164" t="inlineStr"/>
+      <c r="C164" t="n">
+        <v>125</v>
+      </c>
       <c r="D164" t="inlineStr">
         <is>
           <t>item D</t>
@@ -3736,7 +4062,9 @@
       <c r="B165" s="2" t="n">
         <v>44400</v>
       </c>
-      <c r="C165" t="inlineStr"/>
+      <c r="C165" t="n">
+        <v>50</v>
+      </c>
       <c r="D165" t="inlineStr">
         <is>
           <t>item A</t>
@@ -3756,7 +4084,9 @@
       <c r="B166" s="2" t="n">
         <v>44400</v>
       </c>
-      <c r="C166" t="inlineStr"/>
+      <c r="C166" t="n">
+        <v>100</v>
+      </c>
       <c r="D166" t="inlineStr">
         <is>
           <t>item C</t>
@@ -3776,7 +4106,9 @@
       <c r="B167" s="2" t="n">
         <v>44400</v>
       </c>
-      <c r="C167" t="inlineStr"/>
+      <c r="C167" t="n">
+        <v>30</v>
+      </c>
       <c r="D167" t="inlineStr">
         <is>
           <t>item A</t>
@@ -3796,7 +4128,9 @@
       <c r="B168" s="2" t="n">
         <v>44400</v>
       </c>
-      <c r="C168" t="inlineStr"/>
+      <c r="C168" t="n">
+        <v>80</v>
+      </c>
       <c r="D168" t="inlineStr">
         <is>
           <t>item C</t>
@@ -3816,7 +4150,9 @@
       <c r="B169" s="2" t="n">
         <v>44400</v>
       </c>
-      <c r="C169" t="inlineStr"/>
+      <c r="C169" t="n">
+        <v>125</v>
+      </c>
       <c r="D169" t="inlineStr">
         <is>
           <t>item D</t>
@@ -3836,7 +4172,9 @@
       <c r="B170" s="2" t="n">
         <v>44401</v>
       </c>
-      <c r="C170" t="inlineStr"/>
+      <c r="C170" t="n">
+        <v>15</v>
+      </c>
       <c r="D170" t="inlineStr">
         <is>
           <t>item B</t>
@@ -3856,7 +4194,9 @@
       <c r="B171" s="2" t="n">
         <v>44401</v>
       </c>
-      <c r="C171" t="inlineStr"/>
+      <c r="C171" t="n">
+        <v>50</v>
+      </c>
       <c r="D171" t="inlineStr">
         <is>
           <t>item A</t>
@@ -3876,7 +4216,9 @@
       <c r="B172" s="2" t="n">
         <v>44401</v>
       </c>
-      <c r="C172" t="inlineStr"/>
+      <c r="C172" t="n">
+        <v>100</v>
+      </c>
       <c r="D172" t="inlineStr">
         <is>
           <t>item D</t>
@@ -3896,7 +4238,9 @@
       <c r="B173" s="2" t="n">
         <v>44401</v>
       </c>
-      <c r="C173" t="inlineStr"/>
+      <c r="C173" t="n">
+        <v>15</v>
+      </c>
       <c r="D173" t="inlineStr">
         <is>
           <t>item B</t>
@@ -3916,7 +4260,9 @@
       <c r="B174" s="2" t="n">
         <v>44401</v>
       </c>
-      <c r="C174" t="inlineStr"/>
+      <c r="C174" t="n">
+        <v>100</v>
+      </c>
       <c r="D174" t="inlineStr">
         <is>
           <t>item C</t>
@@ -3936,7 +4282,9 @@
       <c r="B175" s="2" t="n">
         <v>44402</v>
       </c>
-      <c r="C175" t="inlineStr"/>
+      <c r="C175" t="n">
+        <v>75</v>
+      </c>
       <c r="D175" t="inlineStr">
         <is>
           <t>item D</t>
@@ -3956,7 +4304,9 @@
       <c r="B176" s="2" t="n">
         <v>44402</v>
       </c>
-      <c r="C176" t="inlineStr"/>
+      <c r="C176" t="n">
+        <v>75</v>
+      </c>
       <c r="D176" t="inlineStr">
         <is>
           <t>item B</t>
@@ -3976,7 +4326,9 @@
       <c r="B177" s="2" t="n">
         <v>44402</v>
       </c>
-      <c r="C177" t="inlineStr"/>
+      <c r="C177" t="n">
+        <v>25</v>
+      </c>
       <c r="D177" t="inlineStr">
         <is>
           <t>item D</t>
@@ -3996,7 +4348,9 @@
       <c r="B178" s="2" t="n">
         <v>44402</v>
       </c>
-      <c r="C178" t="inlineStr"/>
+      <c r="C178" t="n">
+        <v>100</v>
+      </c>
       <c r="D178" t="inlineStr">
         <is>
           <t>item C</t>
@@ -4016,7 +4370,9 @@
       <c r="B179" s="2" t="n">
         <v>44402</v>
       </c>
-      <c r="C179" t="inlineStr"/>
+      <c r="C179" t="n">
+        <v>75</v>
+      </c>
       <c r="D179" t="inlineStr">
         <is>
           <t>item B</t>
@@ -4036,7 +4392,9 @@
       <c r="B180" s="2" t="n">
         <v>44403</v>
       </c>
-      <c r="C180" t="inlineStr"/>
+      <c r="C180" t="n">
+        <v>50</v>
+      </c>
       <c r="D180" t="inlineStr">
         <is>
           <t>item D</t>
@@ -4056,7 +4414,9 @@
       <c r="B181" s="2" t="n">
         <v>44403</v>
       </c>
-      <c r="C181" t="inlineStr"/>
+      <c r="C181" t="n">
+        <v>30</v>
+      </c>
       <c r="D181" t="inlineStr">
         <is>
           <t>item A</t>
@@ -4076,7 +4436,9 @@
       <c r="B182" s="2" t="n">
         <v>44404</v>
       </c>
-      <c r="C182" t="inlineStr"/>
+      <c r="C182" t="n">
+        <v>30</v>
+      </c>
       <c r="D182" t="inlineStr">
         <is>
           <t>item A</t>
@@ -4096,7 +4458,9 @@
       <c r="B183" s="2" t="n">
         <v>44404</v>
       </c>
-      <c r="C183" t="inlineStr"/>
+      <c r="C183" t="n">
+        <v>75</v>
+      </c>
       <c r="D183" t="inlineStr">
         <is>
           <t>item D</t>
@@ -4116,7 +4480,9 @@
       <c r="B184" s="2" t="n">
         <v>44405</v>
       </c>
-      <c r="C184" t="inlineStr"/>
+      <c r="C184" t="n">
+        <v>60</v>
+      </c>
       <c r="D184" t="inlineStr">
         <is>
           <t>item B</t>
@@ -4136,7 +4502,9 @@
       <c r="B185" s="2" t="n">
         <v>44405</v>
       </c>
-      <c r="C185" t="inlineStr"/>
+      <c r="C185" t="n">
+        <v>125</v>
+      </c>
       <c r="D185" t="inlineStr">
         <is>
           <t>item D</t>
@@ -4156,7 +4524,9 @@
       <c r="B186" s="2" t="n">
         <v>44405</v>
       </c>
-      <c r="C186" t="inlineStr"/>
+      <c r="C186" t="n">
+        <v>75</v>
+      </c>
       <c r="D186" t="inlineStr">
         <is>
           <t>item B</t>
@@ -4176,7 +4546,9 @@
       <c r="B187" s="2" t="n">
         <v>44406</v>
       </c>
-      <c r="C187" t="inlineStr"/>
+      <c r="C187" t="n">
+        <v>20</v>
+      </c>
       <c r="D187" t="inlineStr">
         <is>
           <t>item C</t>
@@ -4196,7 +4568,9 @@
       <c r="B188" s="2" t="n">
         <v>44406</v>
       </c>
-      <c r="C188" t="inlineStr"/>
+      <c r="C188" t="n">
+        <v>30</v>
+      </c>
       <c r="D188" t="inlineStr">
         <is>
           <t>item A</t>
@@ -4216,7 +4590,9 @@
       <c r="B189" s="2" t="n">
         <v>44406</v>
       </c>
-      <c r="C189" t="inlineStr"/>
+      <c r="C189" t="n">
+        <v>30</v>
+      </c>
       <c r="D189" t="inlineStr">
         <is>
           <t>item B</t>
@@ -4236,7 +4612,9 @@
       <c r="B190" s="2" t="n">
         <v>44407</v>
       </c>
-      <c r="C190" t="inlineStr"/>
+      <c r="C190" t="n">
+        <v>45</v>
+      </c>
       <c r="D190" t="inlineStr">
         <is>
           <t>item B</t>
@@ -4256,7 +4634,9 @@
       <c r="B191" s="2" t="n">
         <v>44407</v>
       </c>
-      <c r="C191" t="inlineStr"/>
+      <c r="C191" t="n">
+        <v>50</v>
+      </c>
       <c r="D191" t="inlineStr">
         <is>
           <t>item D</t>
@@ -4276,7 +4656,9 @@
       <c r="B192" s="2" t="n">
         <v>44407</v>
       </c>
-      <c r="C192" t="inlineStr"/>
+      <c r="C192" t="n">
+        <v>20</v>
+      </c>
       <c r="D192" t="inlineStr">
         <is>
           <t>item A</t>
@@ -4296,7 +4678,9 @@
       <c r="B193" s="2" t="n">
         <v>44408</v>
       </c>
-      <c r="C193" t="inlineStr"/>
+      <c r="C193" t="n">
+        <v>20</v>
+      </c>
       <c r="D193" t="inlineStr">
         <is>
           <t>item A</t>
@@ -4316,7 +4700,9 @@
       <c r="B194" s="2" t="n">
         <v>44408</v>
       </c>
-      <c r="C194" t="inlineStr"/>
+      <c r="C194" t="n">
+        <v>25</v>
+      </c>
       <c r="D194" t="inlineStr">
         <is>
           <t>item D</t>
@@ -4336,7 +4722,9 @@
       <c r="B195" s="2" t="n">
         <v>44408</v>
       </c>
-      <c r="C195" t="inlineStr"/>
+      <c r="C195" t="n">
+        <v>40</v>
+      </c>
       <c r="D195" t="inlineStr">
         <is>
           <t>item C</t>
@@ -4356,7 +4744,9 @@
       <c r="B196" s="2" t="n">
         <v>44408</v>
       </c>
-      <c r="C196" t="inlineStr"/>
+      <c r="C196" t="n">
+        <v>25</v>
+      </c>
       <c r="D196" t="inlineStr">
         <is>
           <t>item D</t>
@@ -4376,7 +4766,9 @@
       <c r="B197" s="2" t="n">
         <v>44408</v>
       </c>
-      <c r="C197" t="inlineStr"/>
+      <c r="C197" t="n">
+        <v>15</v>
+      </c>
       <c r="D197" t="inlineStr">
         <is>
           <t>item B</t>
@@ -4396,7 +4788,9 @@
       <c r="B198" s="2" t="n">
         <v>44408</v>
       </c>
-      <c r="C198" t="inlineStr"/>
+      <c r="C198" t="n">
+        <v>100</v>
+      </c>
       <c r="D198" t="inlineStr">
         <is>
           <t>item C</t>
@@ -4416,7 +4810,9 @@
       <c r="B199" s="2" t="n">
         <v>44409</v>
       </c>
-      <c r="C199" t="inlineStr"/>
+      <c r="C199" t="n">
+        <v>125</v>
+      </c>
       <c r="D199" t="inlineStr">
         <is>
           <t>item D</t>
@@ -4436,7 +4832,9 @@
       <c r="B200" s="2" t="n">
         <v>44409</v>
       </c>
-      <c r="C200" t="inlineStr"/>
+      <c r="C200" t="n">
+        <v>75</v>
+      </c>
       <c r="D200" t="inlineStr">
         <is>
           <t>item B</t>
@@ -4456,7 +4854,9 @@
       <c r="B201" s="2" t="n">
         <v>44409</v>
       </c>
-      <c r="C201" t="inlineStr"/>
+      <c r="C201" t="n">
+        <v>100</v>
+      </c>
       <c r="D201" t="inlineStr">
         <is>
           <t>item C</t>
@@ -4476,7 +4876,9 @@
       <c r="B202" s="2" t="n">
         <v>44409</v>
       </c>
-      <c r="C202" t="inlineStr"/>
+      <c r="C202" t="n">
+        <v>50</v>
+      </c>
       <c r="D202" t="inlineStr">
         <is>
           <t>item A</t>
@@ -4496,7 +4898,9 @@
       <c r="B203" s="2" t="n">
         <v>44409</v>
       </c>
-      <c r="C203" t="inlineStr"/>
+      <c r="C203" t="n">
+        <v>80</v>
+      </c>
       <c r="D203" t="inlineStr">
         <is>
           <t>item C</t>
@@ -4516,7 +4920,9 @@
       <c r="B204" s="2" t="n">
         <v>44409</v>
       </c>
-      <c r="C204" t="inlineStr"/>
+      <c r="C204" t="n">
+        <v>45</v>
+      </c>
       <c r="D204" t="inlineStr">
         <is>
           <t>item B</t>
@@ -4536,7 +4942,9 @@
       <c r="B205" s="2" t="n">
         <v>44413</v>
       </c>
-      <c r="C205" t="inlineStr"/>
+      <c r="C205" t="n">
+        <v>45</v>
+      </c>
       <c r="D205" t="inlineStr">
         <is>
           <t>item B</t>
@@ -4556,7 +4964,9 @@
       <c r="B206" s="2" t="n">
         <v>44413</v>
       </c>
-      <c r="C206" t="inlineStr"/>
+      <c r="C206" t="n">
+        <v>80</v>
+      </c>
       <c r="D206" t="inlineStr">
         <is>
           <t>item C</t>
@@ -4576,7 +4986,9 @@
       <c r="B207" s="2" t="n">
         <v>44413</v>
       </c>
-      <c r="C207" t="inlineStr"/>
+      <c r="C207" t="n">
+        <v>75</v>
+      </c>
       <c r="D207" t="inlineStr">
         <is>
           <t>item D</t>
@@ -4596,7 +5008,9 @@
       <c r="B208" s="2" t="n">
         <v>44414</v>
       </c>
-      <c r="C208" t="inlineStr"/>
+      <c r="C208" t="n">
+        <v>45</v>
+      </c>
       <c r="D208" t="inlineStr">
         <is>
           <t>item B</t>
@@ -4616,7 +5030,9 @@
       <c r="B209" s="2" t="n">
         <v>44414</v>
       </c>
-      <c r="C209" t="inlineStr"/>
+      <c r="C209" t="n">
+        <v>100</v>
+      </c>
       <c r="D209" t="inlineStr">
         <is>
           <t>item D</t>
@@ -4636,7 +5052,9 @@
       <c r="B210" s="2" t="n">
         <v>44414</v>
       </c>
-      <c r="C210" t="inlineStr"/>
+      <c r="C210" t="n">
+        <v>40</v>
+      </c>
       <c r="D210" t="inlineStr">
         <is>
           <t>item C</t>
@@ -4656,7 +5074,9 @@
       <c r="B211" s="2" t="n">
         <v>44414</v>
       </c>
-      <c r="C211" t="inlineStr"/>
+      <c r="C211" t="n">
+        <v>50</v>
+      </c>
       <c r="D211" t="inlineStr">
         <is>
           <t>item D</t>
@@ -4676,7 +5096,9 @@
       <c r="B212" s="2" t="n">
         <v>44414</v>
       </c>
-      <c r="C212" t="inlineStr"/>
+      <c r="C212" t="n">
+        <v>20</v>
+      </c>
       <c r="D212" t="inlineStr">
         <is>
           <t>item C</t>
@@ -4696,7 +5118,9 @@
       <c r="B213" s="2" t="n">
         <v>44414</v>
       </c>
-      <c r="C213" t="inlineStr"/>
+      <c r="C213" t="n">
+        <v>75</v>
+      </c>
       <c r="D213" t="inlineStr">
         <is>
           <t>item D</t>
@@ -4716,7 +5140,9 @@
       <c r="B214" s="2" t="n">
         <v>44415</v>
       </c>
-      <c r="C214" t="inlineStr"/>
+      <c r="C214" t="n">
+        <v>60</v>
+      </c>
       <c r="D214" t="inlineStr">
         <is>
           <t>item C</t>
@@ -4736,7 +5162,9 @@
       <c r="B215" s="2" t="n">
         <v>44415</v>
       </c>
-      <c r="C215" t="inlineStr"/>
+      <c r="C215" t="n">
+        <v>10</v>
+      </c>
       <c r="D215" t="inlineStr">
         <is>
           <t>item A</t>
@@ -4756,7 +5184,9 @@
       <c r="B216" s="2" t="n">
         <v>44415</v>
       </c>
-      <c r="C216" t="inlineStr"/>
+      <c r="C216" t="n">
+        <v>40</v>
+      </c>
       <c r="D216" t="inlineStr">
         <is>
           <t>item C</t>
@@ -4776,7 +5206,9 @@
       <c r="B217" s="2" t="n">
         <v>44415</v>
       </c>
-      <c r="C217" t="inlineStr"/>
+      <c r="C217" t="n">
+        <v>125</v>
+      </c>
       <c r="D217" t="inlineStr">
         <is>
           <t>item D</t>
@@ -4796,7 +5228,9 @@
       <c r="B218" s="2" t="n">
         <v>44415</v>
       </c>
-      <c r="C218" t="inlineStr"/>
+      <c r="C218" t="n">
+        <v>40</v>
+      </c>
       <c r="D218" t="inlineStr">
         <is>
           <t>item A</t>
@@ -4816,7 +5250,9 @@
       <c r="B219" s="2" t="n">
         <v>44416</v>
       </c>
-      <c r="C219" t="inlineStr"/>
+      <c r="C219" t="n">
+        <v>60</v>
+      </c>
       <c r="D219" t="inlineStr">
         <is>
           <t>item C</t>
@@ -4836,7 +5272,9 @@
       <c r="B220" s="2" t="n">
         <v>44416</v>
       </c>
-      <c r="C220" t="inlineStr"/>
+      <c r="C220" t="n">
+        <v>20</v>
+      </c>
       <c r="D220" t="inlineStr">
         <is>
           <t>item A</t>
@@ -4856,7 +5294,9 @@
       <c r="B221" s="2" t="n">
         <v>44416</v>
       </c>
-      <c r="C221" t="inlineStr"/>
+      <c r="C221" t="n">
+        <v>20</v>
+      </c>
       <c r="D221" t="inlineStr">
         <is>
           <t>item C</t>
@@ -4876,7 +5316,9 @@
       <c r="B222" s="2" t="n">
         <v>44416</v>
       </c>
-      <c r="C222" t="inlineStr"/>
+      <c r="C222" t="n">
+        <v>15</v>
+      </c>
       <c r="D222" t="inlineStr">
         <is>
           <t>item B</t>
@@ -4896,7 +5338,9 @@
       <c r="B223" s="2" t="n">
         <v>44416</v>
       </c>
-      <c r="C223" t="inlineStr"/>
+      <c r="C223" t="n">
+        <v>30</v>
+      </c>
       <c r="D223" t="inlineStr">
         <is>
           <t>item A</t>
@@ -4916,7 +5360,9 @@
       <c r="B224" s="2" t="n">
         <v>44416</v>
       </c>
-      <c r="C224" t="inlineStr"/>
+      <c r="C224" t="n">
+        <v>60</v>
+      </c>
       <c r="D224" t="inlineStr">
         <is>
           <t>item C</t>
@@ -4936,7 +5382,9 @@
       <c r="B225" s="2" t="n">
         <v>44418</v>
       </c>
-      <c r="C225" t="inlineStr"/>
+      <c r="C225" t="n">
+        <v>125</v>
+      </c>
       <c r="D225" t="inlineStr">
         <is>
           <t>item D</t>
@@ -4956,7 +5404,9 @@
       <c r="B226" s="2" t="n">
         <v>44418</v>
       </c>
-      <c r="C226" t="inlineStr"/>
+      <c r="C226" t="n">
+        <v>30</v>
+      </c>
       <c r="D226" t="inlineStr">
         <is>
           <t>item B</t>
@@ -4976,7 +5426,9 @@
       <c r="B227" s="2" t="n">
         <v>44420</v>
       </c>
-      <c r="C227" t="inlineStr"/>
+      <c r="C227" t="n">
+        <v>125</v>
+      </c>
       <c r="D227" t="inlineStr">
         <is>
           <t>item D</t>
@@ -4996,7 +5448,9 @@
       <c r="B228" s="2" t="n">
         <v>44420</v>
       </c>
-      <c r="C228" t="inlineStr"/>
+      <c r="C228" t="n">
+        <v>50</v>
+      </c>
       <c r="D228" t="inlineStr">
         <is>
           <t>item A</t>
@@ -5016,7 +5470,9 @@
       <c r="B229" s="2" t="n">
         <v>44420</v>
       </c>
-      <c r="C229" t="inlineStr"/>
+      <c r="C229" t="n">
+        <v>20</v>
+      </c>
       <c r="D229" t="inlineStr">
         <is>
           <t>item C</t>
@@ -5036,7 +5492,9 @@
       <c r="B230" s="2" t="n">
         <v>44421</v>
       </c>
-      <c r="C230" t="inlineStr"/>
+      <c r="C230" t="n">
+        <v>20</v>
+      </c>
       <c r="D230" t="inlineStr">
         <is>
           <t>item C</t>
@@ -5056,7 +5514,9 @@
       <c r="B231" s="2" t="n">
         <v>44421</v>
       </c>
-      <c r="C231" t="inlineStr"/>
+      <c r="C231" t="n">
+        <v>45</v>
+      </c>
       <c r="D231" t="inlineStr">
         <is>
           <t>item B</t>
@@ -5076,7 +5536,9 @@
       <c r="B232" s="2" t="n">
         <v>44421</v>
       </c>
-      <c r="C232" t="inlineStr"/>
+      <c r="C232" t="n">
+        <v>20</v>
+      </c>
       <c r="D232" t="inlineStr">
         <is>
           <t>item C</t>
@@ -5096,7 +5558,9 @@
       <c r="B233" s="2" t="n">
         <v>44421</v>
       </c>
-      <c r="C233" t="inlineStr"/>
+      <c r="C233" t="n">
+        <v>45</v>
+      </c>
       <c r="D233" t="inlineStr">
         <is>
           <t>item B</t>
@@ -5116,7 +5580,9 @@
       <c r="B234" s="2" t="n">
         <v>44421</v>
       </c>
-      <c r="C234" t="inlineStr"/>
+      <c r="C234" t="n">
+        <v>100</v>
+      </c>
       <c r="D234" t="inlineStr">
         <is>
           <t>item C</t>
@@ -5136,7 +5602,9 @@
       <c r="B235" s="2" t="n">
         <v>44421</v>
       </c>
-      <c r="C235" t="inlineStr"/>
+      <c r="C235" t="n">
+        <v>40</v>
+      </c>
       <c r="D235" t="inlineStr">
         <is>
           <t>item A</t>
@@ -5156,7 +5624,9 @@
       <c r="B236" s="2" t="n">
         <v>44422</v>
       </c>
-      <c r="C236" t="inlineStr"/>
+      <c r="C236" t="n">
+        <v>15</v>
+      </c>
       <c r="D236" t="inlineStr">
         <is>
           <t>item B</t>
@@ -5176,7 +5646,9 @@
       <c r="B237" s="2" t="n">
         <v>44422</v>
       </c>
-      <c r="C237" t="inlineStr"/>
+      <c r="C237" t="n">
+        <v>50</v>
+      </c>
       <c r="D237" t="inlineStr">
         <is>
           <t>item A</t>
@@ -5196,7 +5668,9 @@
       <c r="B238" s="2" t="n">
         <v>44422</v>
       </c>
-      <c r="C238" t="inlineStr"/>
+      <c r="C238" t="n">
+        <v>60</v>
+      </c>
       <c r="D238" t="inlineStr">
         <is>
           <t>item B</t>
@@ -5216,7 +5690,9 @@
       <c r="B239" s="2" t="n">
         <v>44422</v>
       </c>
-      <c r="C239" t="inlineStr"/>
+      <c r="C239" t="n">
+        <v>40</v>
+      </c>
       <c r="D239" t="inlineStr">
         <is>
           <t>item A</t>
@@ -5236,7 +5712,9 @@
       <c r="B240" s="2" t="n">
         <v>44423</v>
       </c>
-      <c r="C240" t="inlineStr"/>
+      <c r="C240" t="n">
+        <v>40</v>
+      </c>
       <c r="D240" t="inlineStr">
         <is>
           <t>item A</t>
@@ -5256,7 +5734,9 @@
       <c r="B241" s="2" t="n">
         <v>44423</v>
       </c>
-      <c r="C241" t="inlineStr"/>
+      <c r="C241" t="n">
+        <v>100</v>
+      </c>
       <c r="D241" t="inlineStr">
         <is>
           <t>item D</t>
@@ -5276,7 +5756,9 @@
       <c r="B242" s="2" t="n">
         <v>44423</v>
       </c>
-      <c r="C242" t="inlineStr"/>
+      <c r="C242" t="n">
+        <v>30</v>
+      </c>
       <c r="D242" t="inlineStr">
         <is>
           <t>item B</t>
@@ -5296,7 +5778,9 @@
       <c r="B243" s="2" t="n">
         <v>44423</v>
       </c>
-      <c r="C243" t="inlineStr"/>
+      <c r="C243" t="n">
+        <v>20</v>
+      </c>
       <c r="D243" t="inlineStr">
         <is>
           <t>item C</t>
@@ -5316,7 +5800,9 @@
       <c r="B244" s="2" t="n">
         <v>44423</v>
       </c>
-      <c r="C244" t="inlineStr"/>
+      <c r="C244" t="n">
+        <v>10</v>
+      </c>
       <c r="D244" t="inlineStr">
         <is>
           <t>item A</t>
@@ -5336,7 +5822,9 @@
       <c r="B245" s="2" t="n">
         <v>44423</v>
       </c>
-      <c r="C245" t="inlineStr"/>
+      <c r="C245" t="n">
+        <v>100</v>
+      </c>
       <c r="D245" t="inlineStr">
         <is>
           <t>item D</t>
@@ -5356,7 +5844,9 @@
       <c r="B246" s="2" t="n">
         <v>44424</v>
       </c>
-      <c r="C246" t="inlineStr"/>
+      <c r="C246" t="n">
+        <v>40</v>
+      </c>
       <c r="D246" t="inlineStr">
         <is>
           <t>item A</t>
@@ -5376,7 +5866,9 @@
       <c r="B247" s="2" t="n">
         <v>44424</v>
       </c>
-      <c r="C247" t="inlineStr"/>
+      <c r="C247" t="n">
+        <v>25</v>
+      </c>
       <c r="D247" t="inlineStr">
         <is>
           <t>item D</t>
@@ -5396,7 +5888,9 @@
       <c r="B248" s="2" t="n">
         <v>44424</v>
       </c>
-      <c r="C248" t="inlineStr"/>
+      <c r="C248" t="n">
+        <v>60</v>
+      </c>
       <c r="D248" t="inlineStr">
         <is>
           <t>item B</t>
@@ -5416,7 +5910,9 @@
       <c r="B249" s="2" t="n">
         <v>44425</v>
       </c>
-      <c r="C249" t="inlineStr"/>
+      <c r="C249" t="n">
+        <v>40</v>
+      </c>
       <c r="D249" t="inlineStr">
         <is>
           <t>item A</t>
@@ -5436,7 +5932,9 @@
       <c r="B250" s="2" t="n">
         <v>44425</v>
       </c>
-      <c r="C250" t="inlineStr"/>
+      <c r="C250" t="n">
+        <v>60</v>
+      </c>
       <c r="D250" t="inlineStr">
         <is>
           <t>item B</t>
@@ -5456,7 +5954,9 @@
       <c r="B251" s="2" t="n">
         <v>44426</v>
       </c>
-      <c r="C251" t="inlineStr"/>
+      <c r="C251" t="n">
+        <v>50</v>
+      </c>
       <c r="D251" t="inlineStr">
         <is>
           <t>item D</t>
@@ -5476,7 +5976,9 @@
       <c r="B252" s="2" t="n">
         <v>44426</v>
       </c>
-      <c r="C252" t="inlineStr"/>
+      <c r="C252" t="n">
+        <v>80</v>
+      </c>
       <c r="D252" t="inlineStr">
         <is>
           <t>item C</t>
@@ -5496,7 +5998,9 @@
       <c r="B253" s="2" t="n">
         <v>44427</v>
       </c>
-      <c r="C253" t="inlineStr"/>
+      <c r="C253" t="n">
+        <v>100</v>
+      </c>
       <c r="D253" t="inlineStr">
         <is>
           <t>item C</t>
@@ -5516,7 +6020,9 @@
       <c r="B254" s="2" t="n">
         <v>44427</v>
       </c>
-      <c r="C254" t="inlineStr"/>
+      <c r="C254" t="n">
+        <v>45</v>
+      </c>
       <c r="D254" t="inlineStr">
         <is>
           <t>item B</t>
@@ -5536,7 +6042,9 @@
       <c r="B255" s="2" t="n">
         <v>44428</v>
       </c>
-      <c r="C255" t="inlineStr"/>
+      <c r="C255" t="n">
+        <v>75</v>
+      </c>
       <c r="D255" t="inlineStr">
         <is>
           <t>item B</t>
@@ -5556,7 +6064,9 @@
       <c r="B256" s="2" t="n">
         <v>44428</v>
       </c>
-      <c r="C256" t="inlineStr"/>
+      <c r="C256" t="n">
+        <v>60</v>
+      </c>
       <c r="D256" t="inlineStr">
         <is>
           <t>item C</t>
@@ -5576,7 +6086,9 @@
       <c r="B257" s="2" t="n">
         <v>44428</v>
       </c>
-      <c r="C257" t="inlineStr"/>
+      <c r="C257" t="n">
+        <v>50</v>
+      </c>
       <c r="D257" t="inlineStr">
         <is>
           <t>item A</t>
@@ -5596,7 +6108,9 @@
       <c r="B258" s="2" t="n">
         <v>44428</v>
       </c>
-      <c r="C258" t="inlineStr"/>
+      <c r="C258" t="n">
+        <v>50</v>
+      </c>
       <c r="D258" t="inlineStr">
         <is>
           <t>item D</t>
@@ -5616,7 +6130,9 @@
       <c r="B259" s="2" t="n">
         <v>44429</v>
       </c>
-      <c r="C259" t="inlineStr"/>
+      <c r="C259" t="n">
+        <v>100</v>
+      </c>
       <c r="D259" t="inlineStr">
         <is>
           <t>item D</t>
@@ -5636,7 +6152,9 @@
       <c r="B260" s="2" t="n">
         <v>44429</v>
       </c>
-      <c r="C260" t="inlineStr"/>
+      <c r="C260" t="n">
+        <v>50</v>
+      </c>
       <c r="D260" t="inlineStr">
         <is>
           <t>item A</t>
@@ -5656,7 +6174,9 @@
       <c r="B261" s="2" t="n">
         <v>44429</v>
       </c>
-      <c r="C261" t="inlineStr"/>
+      <c r="C261" t="n">
+        <v>125</v>
+      </c>
       <c r="D261" t="inlineStr">
         <is>
           <t>item D</t>
@@ -5676,7 +6196,9 @@
       <c r="B262" s="2" t="n">
         <v>44429</v>
       </c>
-      <c r="C262" t="inlineStr"/>
+      <c r="C262" t="n">
+        <v>80</v>
+      </c>
       <c r="D262" t="inlineStr">
         <is>
           <t>item C</t>
@@ -5696,7 +6218,9 @@
       <c r="B263" s="2" t="n">
         <v>44430</v>
       </c>
-      <c r="C263" t="inlineStr"/>
+      <c r="C263" t="n">
+        <v>30</v>
+      </c>
       <c r="D263" t="inlineStr">
         <is>
           <t>item B</t>
@@ -5716,7 +6240,9 @@
       <c r="B264" s="2" t="n">
         <v>44430</v>
       </c>
-      <c r="C264" t="inlineStr"/>
+      <c r="C264" t="n">
+        <v>100</v>
+      </c>
       <c r="D264" t="inlineStr">
         <is>
           <t>item D</t>
@@ -5736,7 +6262,9 @@
       <c r="B265" s="2" t="n">
         <v>44430</v>
       </c>
-      <c r="C265" t="inlineStr"/>
+      <c r="C265" t="n">
+        <v>10</v>
+      </c>
       <c r="D265" t="inlineStr">
         <is>
           <t>item A</t>
@@ -5756,7 +6284,9 @@
       <c r="B266" s="2" t="n">
         <v>44430</v>
       </c>
-      <c r="C266" t="inlineStr"/>
+      <c r="C266" t="n">
+        <v>100</v>
+      </c>
       <c r="D266" t="inlineStr">
         <is>
           <t>item C</t>
@@ -5776,7 +6306,9 @@
       <c r="B267" s="2" t="n">
         <v>44431</v>
       </c>
-      <c r="C267" t="inlineStr"/>
+      <c r="C267" t="n">
+        <v>45</v>
+      </c>
       <c r="D267" t="inlineStr">
         <is>
           <t>item B</t>
@@ -5796,7 +6328,9 @@
       <c r="B268" s="2" t="n">
         <v>44431</v>
       </c>
-      <c r="C268" t="inlineStr"/>
+      <c r="C268" t="n">
+        <v>10</v>
+      </c>
       <c r="D268" t="inlineStr">
         <is>
           <t>item A</t>
@@ -5816,7 +6350,9 @@
       <c r="B269" s="2" t="n">
         <v>44431</v>
       </c>
-      <c r="C269" t="inlineStr"/>
+      <c r="C269" t="n">
+        <v>25</v>
+      </c>
       <c r="D269" t="inlineStr">
         <is>
           <t>item D</t>
@@ -5836,7 +6372,9 @@
       <c r="B270" s="2" t="n">
         <v>44432</v>
       </c>
-      <c r="C270" t="inlineStr"/>
+      <c r="C270" t="n">
+        <v>100</v>
+      </c>
       <c r="D270" t="inlineStr">
         <is>
           <t>item D</t>
@@ -5856,7 +6394,9 @@
       <c r="B271" s="2" t="n">
         <v>44432</v>
       </c>
-      <c r="C271" t="inlineStr"/>
+      <c r="C271" t="n">
+        <v>10</v>
+      </c>
       <c r="D271" t="inlineStr">
         <is>
           <t>item A</t>
@@ -5876,7 +6416,9 @@
       <c r="B272" s="2" t="n">
         <v>44432</v>
       </c>
-      <c r="C272" t="inlineStr"/>
+      <c r="C272" t="n">
+        <v>75</v>
+      </c>
       <c r="D272" t="inlineStr">
         <is>
           <t>item D</t>
@@ -5896,7 +6438,9 @@
       <c r="B273" s="2" t="n">
         <v>44433</v>
       </c>
-      <c r="C273" t="inlineStr"/>
+      <c r="C273" t="n">
+        <v>60</v>
+      </c>
       <c r="D273" t="inlineStr">
         <is>
           <t>item C</t>
@@ -5916,7 +6460,9 @@
       <c r="B274" s="2" t="n">
         <v>44433</v>
       </c>
-      <c r="C274" t="inlineStr"/>
+      <c r="C274" t="n">
+        <v>25</v>
+      </c>
       <c r="D274" t="inlineStr">
         <is>
           <t>item D</t>
@@ -5936,7 +6482,9 @@
       <c r="B275" s="2" t="n">
         <v>44434</v>
       </c>
-      <c r="C275" t="inlineStr"/>
+      <c r="C275" t="n">
+        <v>40</v>
+      </c>
       <c r="D275" t="inlineStr">
         <is>
           <t>item A</t>
@@ -5956,7 +6504,9 @@
       <c r="B276" s="2" t="n">
         <v>44434</v>
       </c>
-      <c r="C276" t="inlineStr"/>
+      <c r="C276" t="n">
+        <v>20</v>
+      </c>
       <c r="D276" t="inlineStr">
         <is>
           <t>item C</t>
@@ -5976,7 +6526,9 @@
       <c r="B277" s="2" t="n">
         <v>44434</v>
       </c>
-      <c r="C277" t="inlineStr"/>
+      <c r="C277" t="n">
+        <v>15</v>
+      </c>
       <c r="D277" t="inlineStr">
         <is>
           <t>item B</t>
@@ -5996,7 +6548,9 @@
       <c r="B278" s="2" t="n">
         <v>44435</v>
       </c>
-      <c r="C278" t="inlineStr"/>
+      <c r="C278" t="n">
+        <v>20</v>
+      </c>
       <c r="D278" t="inlineStr">
         <is>
           <t>item A</t>
@@ -6016,7 +6570,9 @@
       <c r="B279" s="2" t="n">
         <v>44435</v>
       </c>
-      <c r="C279" t="inlineStr"/>
+      <c r="C279" t="n">
+        <v>30</v>
+      </c>
       <c r="D279" t="inlineStr">
         <is>
           <t>item B</t>
@@ -6036,7 +6592,9 @@
       <c r="B280" s="2" t="n">
         <v>44435</v>
       </c>
-      <c r="C280" t="inlineStr"/>
+      <c r="C280" t="n">
+        <v>50</v>
+      </c>
       <c r="D280" t="inlineStr">
         <is>
           <t>item D</t>
@@ -6056,7 +6614,9 @@
       <c r="B281" s="2" t="n">
         <v>44436</v>
       </c>
-      <c r="C281" t="inlineStr"/>
+      <c r="C281" t="n">
+        <v>100</v>
+      </c>
       <c r="D281" t="inlineStr">
         <is>
           <t>item D</t>
@@ -6076,7 +6636,9 @@
       <c r="B282" s="2" t="n">
         <v>44436</v>
       </c>
-      <c r="C282" t="inlineStr"/>
+      <c r="C282" t="n">
+        <v>10</v>
+      </c>
       <c r="D282" t="inlineStr">
         <is>
           <t>item A</t>
@@ -6096,7 +6658,9 @@
       <c r="B283" s="2" t="n">
         <v>44436</v>
       </c>
-      <c r="C283" t="inlineStr"/>
+      <c r="C283" t="n">
+        <v>20</v>
+      </c>
       <c r="D283" t="inlineStr">
         <is>
           <t>item C</t>
@@ -6116,7 +6680,9 @@
       <c r="B284" s="2" t="n">
         <v>44437</v>
       </c>
-      <c r="C284" t="inlineStr"/>
+      <c r="C284" t="n">
+        <v>100</v>
+      </c>
       <c r="D284" t="inlineStr">
         <is>
           <t>item D</t>
@@ -6136,7 +6702,9 @@
       <c r="B285" s="2" t="n">
         <v>44437</v>
       </c>
-      <c r="C285" t="inlineStr"/>
+      <c r="C285" t="n">
+        <v>60</v>
+      </c>
       <c r="D285" t="inlineStr">
         <is>
           <t>item C</t>
@@ -6156,7 +6724,9 @@
       <c r="B286" s="2" t="n">
         <v>44437</v>
       </c>
-      <c r="C286" t="inlineStr"/>
+      <c r="C286" t="n">
+        <v>30</v>
+      </c>
       <c r="D286" t="inlineStr">
         <is>
           <t>item A</t>
@@ -6176,7 +6746,9 @@
       <c r="B287" s="2" t="n">
         <v>44437</v>
       </c>
-      <c r="C287" t="inlineStr"/>
+      <c r="C287" t="n">
+        <v>15</v>
+      </c>
       <c r="D287" t="inlineStr">
         <is>
           <t>item B</t>
@@ -6196,7 +6768,9 @@
       <c r="B288" s="2" t="n">
         <v>44437</v>
       </c>
-      <c r="C288" t="inlineStr"/>
+      <c r="C288" t="n">
+        <v>50</v>
+      </c>
       <c r="D288" t="inlineStr">
         <is>
           <t>item D</t>
@@ -6216,7 +6790,9 @@
       <c r="B289" s="2" t="n">
         <v>44438</v>
       </c>
-      <c r="C289" t="inlineStr"/>
+      <c r="C289" t="n">
+        <v>40</v>
+      </c>
       <c r="D289" t="inlineStr">
         <is>
           <t>item A</t>
@@ -6236,7 +6812,9 @@
       <c r="B290" s="2" t="n">
         <v>44438</v>
       </c>
-      <c r="C290" t="inlineStr"/>
+      <c r="C290" t="n">
+        <v>75</v>
+      </c>
       <c r="D290" t="inlineStr">
         <is>
           <t>item D</t>
@@ -6256,7 +6834,9 @@
       <c r="B291" s="2" t="n">
         <v>44439</v>
       </c>
-      <c r="C291" t="inlineStr"/>
+      <c r="C291" t="n">
+        <v>75</v>
+      </c>
       <c r="D291" t="inlineStr">
         <is>
           <t>item D</t>
@@ -6276,7 +6856,9 @@
       <c r="B292" s="2" t="n">
         <v>44439</v>
       </c>
-      <c r="C292" t="inlineStr"/>
+      <c r="C292" t="n">
+        <v>100</v>
+      </c>
       <c r="D292" t="inlineStr">
         <is>
           <t>item C</t>
@@ -6296,7 +6878,9 @@
       <c r="B293" s="2" t="n">
         <v>44439</v>
       </c>
-      <c r="C293" t="inlineStr"/>
+      <c r="C293" t="n">
+        <v>30</v>
+      </c>
       <c r="D293" t="inlineStr">
         <is>
           <t>item A</t>
@@ -6316,7 +6900,9 @@
       <c r="B294" s="2" t="n">
         <v>44440</v>
       </c>
-      <c r="C294" t="inlineStr"/>
+      <c r="C294" t="n">
+        <v>50</v>
+      </c>
       <c r="D294" t="inlineStr">
         <is>
           <t>item D</t>
@@ -6336,7 +6922,9 @@
       <c r="B295" s="2" t="n">
         <v>44440</v>
       </c>
-      <c r="C295" t="inlineStr"/>
+      <c r="C295" t="n">
+        <v>10</v>
+      </c>
       <c r="D295" t="inlineStr">
         <is>
           <t>item A</t>
@@ -6356,7 +6944,9 @@
       <c r="B296" s="2" t="n">
         <v>44440</v>
       </c>
-      <c r="C296" t="inlineStr"/>
+      <c r="C296" t="n">
+        <v>80</v>
+      </c>
       <c r="D296" t="inlineStr">
         <is>
           <t>item C</t>

</xml_diff>